<commit_message>
After removing artifacts from the last merge
</commit_message>
<xml_diff>
--- a/tutorial/inputs/scenarios_list.xlsx
+++ b/tutorial/inputs/scenarios_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="501">
   <si>
     <t>input_file</t>
   </si>
@@ -2162,7 +2162,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2342,9 +2342,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="51" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="52" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2721,13 +2718,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G204"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B177" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G193" sqref="G193"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2736,10 +2733,10 @@
     <col min="2" max="2" width="64.77734375" customWidth="1"/>
     <col min="3" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="4" width="17" style="38" customWidth="1"/>
-    <col min="5" max="7" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>94</v>
       </c>
@@ -2755,14 +2752,8 @@
       <c r="E1" s="87">
         <v>208</v>
       </c>
-      <c r="F1" s="87">
-        <v>209</v>
-      </c>
-      <c r="G1" s="87">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2778,14 +2769,8 @@
       <c r="E2" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2801,14 +2786,8 @@
       <c r="E3" s="76">
         <v>1</v>
       </c>
-      <c r="F3" s="76">
-        <v>1</v>
-      </c>
-      <c r="G3" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
         <v>454</v>
       </c>
@@ -2824,14 +2803,8 @@
       <c r="E4" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="70" t="s">
         <v>455</v>
       </c>
@@ -2847,14 +2820,8 @@
       <c r="E5" s="76" t="s">
         <v>458</v>
       </c>
-      <c r="F5" s="76" t="s">
-        <v>458</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -2870,14 +2837,8 @@
       <c r="E6" s="76">
         <v>180</v>
       </c>
-      <c r="F6" s="76">
-        <v>180</v>
-      </c>
-      <c r="G6" s="76">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -2893,14 +2854,8 @@
       <c r="E7" s="77">
         <v>4.1666666999999998E-2</v>
       </c>
-      <c r="F7" s="77">
-        <v>4.1666666999999998E-2</v>
-      </c>
-      <c r="G7" s="77">
-        <v>4.1666666999999998E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -2916,14 +2871,8 @@
       <c r="E8" s="77">
         <v>4.1666666999999998E-2</v>
       </c>
-      <c r="F8" s="88">
-        <v>1</v>
-      </c>
-      <c r="G8" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
@@ -2936,17 +2885,11 @@
       <c r="D9" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="89" t="s">
+      <c r="E9" s="88" t="s">
         <v>498</v>
       </c>
-      <c r="F9" s="76" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="76" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2962,14 +2905,8 @@
       <c r="E10" s="76">
         <v>1</v>
       </c>
-      <c r="F10" s="76">
-        <v>1</v>
-      </c>
-      <c r="G10" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>461</v>
       </c>
@@ -2985,14 +2922,8 @@
       <c r="E11" s="76">
         <v>0</v>
       </c>
-      <c r="F11" s="76">
-        <v>0</v>
-      </c>
-      <c r="G11" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
@@ -3008,14 +2939,8 @@
       <c r="E12" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -3031,14 +2956,8 @@
       <c r="E13" s="78">
         <v>5.0000000000000001E-9</v>
       </c>
-      <c r="F13" s="78">
-        <v>5.0000000000000001E-9</v>
-      </c>
-      <c r="G13" s="78">
-        <v>5.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -3054,14 +2973,8 @@
       <c r="E14" s="76">
         <v>10</v>
       </c>
-      <c r="F14" s="76">
-        <v>10</v>
-      </c>
-      <c r="G14" s="76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>479</v>
       </c>
@@ -3077,14 +2990,8 @@
       <c r="E15" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="89" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>480</v>
       </c>
@@ -3100,14 +3007,8 @@
       <c r="E16" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>483</v>
       </c>
@@ -3123,14 +3024,8 @@
       <c r="E17" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>499</v>
       </c>
@@ -3146,14 +3041,8 @@
       <c r="E18" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="89" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>484</v>
       </c>
@@ -3169,14 +3058,8 @@
       <c r="E19" s="76">
         <v>86400</v>
       </c>
-      <c r="F19" s="76">
-        <v>86400</v>
-      </c>
-      <c r="G19" s="76">
-        <v>86400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>10</v>
       </c>
@@ -3192,14 +3075,8 @@
       <c r="E20" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>11</v>
       </c>
@@ -3215,14 +3092,8 @@
       <c r="E21" s="76">
         <v>3</v>
       </c>
-      <c r="F21" s="76">
-        <v>3</v>
-      </c>
-      <c r="G21" s="76">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>362</v>
       </c>
@@ -3238,14 +3109,8 @@
       <c r="E22" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="79" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>364</v>
       </c>
@@ -3261,14 +3126,8 @@
       <c r="E23" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="79" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>376</v>
       </c>
@@ -3284,14 +3143,8 @@
       <c r="E24" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>375</v>
       </c>
@@ -3307,14 +3160,8 @@
       <c r="E25" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G25" s="79" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>374</v>
       </c>
@@ -3330,14 +3177,8 @@
       <c r="E26" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" s="79" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>12</v>
       </c>
@@ -3353,14 +3194,8 @@
       <c r="E27" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>13</v>
       </c>
@@ -3376,14 +3211,8 @@
       <c r="E28" s="76">
         <v>0.33</v>
       </c>
-      <c r="F28" s="76">
-        <v>0.33</v>
-      </c>
-      <c r="G28" s="76">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>14</v>
       </c>
@@ -3399,14 +3228,8 @@
       <c r="E29" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>9</v>
       </c>
@@ -3422,14 +3245,8 @@
       <c r="E30" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>467</v>
       </c>
@@ -3445,14 +3262,8 @@
       <c r="E31" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>21</v>
       </c>
@@ -3468,14 +3279,8 @@
       <c r="E32" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F32" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>22</v>
       </c>
@@ -3491,14 +3296,8 @@
       <c r="E33" s="76" t="s">
         <v>487</v>
       </c>
-      <c r="F33" s="76" t="s">
-        <v>487</v>
-      </c>
-      <c r="G33" s="76" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>23</v>
       </c>
@@ -3514,14 +3313,8 @@
       <c r="E34" s="78">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F34" s="78">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G34" s="78">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>24</v>
       </c>
@@ -3537,14 +3330,8 @@
       <c r="E35" s="78">
         <v>1E-3</v>
       </c>
-      <c r="F35" s="78">
-        <v>1E-3</v>
-      </c>
-      <c r="G35" s="78">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>25</v>
       </c>
@@ -3560,14 +3347,8 @@
       <c r="E36" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F36" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G36" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>26</v>
       </c>
@@ -3583,14 +3364,8 @@
       <c r="E37" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="G37" s="76" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
         <v>27</v>
       </c>
@@ -3606,14 +3381,8 @@
       <c r="E38" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F38" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G38" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
         <v>28</v>
       </c>
@@ -3629,14 +3398,8 @@
       <c r="E39" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G39" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
         <v>29</v>
       </c>
@@ -3652,14 +3415,8 @@
       <c r="E40" s="76">
         <v>120</v>
       </c>
-      <c r="F40" s="76">
-        <v>120</v>
-      </c>
-      <c r="G40" s="76">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
         <v>30</v>
       </c>
@@ -3675,14 +3432,8 @@
       <c r="E41" s="76">
         <v>0</v>
       </c>
-      <c r="F41" s="76">
-        <v>0</v>
-      </c>
-      <c r="G41" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>31</v>
       </c>
@@ -3698,14 +3449,8 @@
       <c r="E42" s="76">
         <v>0</v>
       </c>
-      <c r="F42" s="76">
-        <v>0</v>
-      </c>
-      <c r="G42" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>32</v>
       </c>
@@ -3721,14 +3466,8 @@
       <c r="E43" s="76">
         <v>-0.1</v>
       </c>
-      <c r="F43" s="76">
-        <v>-0.1</v>
-      </c>
-      <c r="G43" s="76">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
         <v>476</v>
       </c>
@@ -3744,14 +3483,8 @@
       <c r="E44" s="76">
         <v>-0.2</v>
       </c>
-      <c r="F44" s="76">
-        <v>-0.2</v>
-      </c>
-      <c r="G44" s="76">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
         <v>477</v>
       </c>
@@ -3767,14 +3500,8 @@
       <c r="E45" s="76">
         <v>-0.2</v>
       </c>
-      <c r="F45" s="76">
-        <v>-0.2</v>
-      </c>
-      <c r="G45" s="76">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
         <v>33</v>
       </c>
@@ -3790,14 +3517,8 @@
       <c r="E46" s="76">
         <v>0.4</v>
       </c>
-      <c r="F46" s="76">
-        <v>0.4</v>
-      </c>
-      <c r="G46" s="76">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
         <v>35</v>
       </c>
@@ -3813,14 +3534,8 @@
       <c r="E47" s="76">
         <v>0</v>
       </c>
-      <c r="F47" s="76">
-        <v>0</v>
-      </c>
-      <c r="G47" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>437</v>
       </c>
@@ -3836,14 +3551,8 @@
       <c r="E48" s="76">
         <v>1200</v>
       </c>
-      <c r="F48" s="76">
-        <v>1200</v>
-      </c>
-      <c r="G48" s="76">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>438</v>
       </c>
@@ -3859,14 +3568,8 @@
       <c r="E49" s="76">
         <v>1200</v>
       </c>
-      <c r="F49" s="76">
-        <v>1200</v>
-      </c>
-      <c r="G49" s="76">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>470</v>
       </c>
@@ -3882,14 +3585,8 @@
       <c r="E50" s="80" t="s">
         <v>472</v>
       </c>
-      <c r="F50" s="80" t="s">
-        <v>472</v>
-      </c>
-      <c r="G50" s="80" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
         <v>15</v>
       </c>
@@ -3905,14 +3602,8 @@
       <c r="E51" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F51" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G51" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>16</v>
       </c>
@@ -3928,14 +3619,8 @@
       <c r="E52" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F52" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G52" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>17</v>
       </c>
@@ -3951,14 +3636,8 @@
       <c r="E53" s="76">
         <v>0</v>
       </c>
-      <c r="F53" s="76">
-        <v>0</v>
-      </c>
-      <c r="G53" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>18</v>
       </c>
@@ -3974,14 +3653,8 @@
       <c r="E54" s="76">
         <v>0.5</v>
       </c>
-      <c r="F54" s="76">
-        <v>0.5</v>
-      </c>
-      <c r="G54" s="76">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>19</v>
       </c>
@@ -3997,14 +3670,8 @@
       <c r="E55" s="76">
         <v>0.05</v>
       </c>
-      <c r="F55" s="76">
-        <v>0.05</v>
-      </c>
-      <c r="G55" s="76">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
         <v>36</v>
       </c>
@@ -4020,14 +3687,8 @@
       <c r="E56" s="78">
         <v>1E-3</v>
       </c>
-      <c r="F56" s="78">
-        <v>1E-3</v>
-      </c>
-      <c r="G56" s="78">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="16" t="s">
         <v>379</v>
       </c>
@@ -4043,14 +3704,8 @@
       <c r="E57" s="76">
         <v>0</v>
       </c>
-      <c r="F57" s="76">
-        <v>0</v>
-      </c>
-      <c r="G57" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
         <v>37</v>
       </c>
@@ -4066,14 +3721,8 @@
       <c r="E58" s="76">
         <v>1E-4</v>
       </c>
-      <c r="F58" s="76">
-        <v>1E-4</v>
-      </c>
-      <c r="G58" s="76">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
         <v>38</v>
       </c>
@@ -4089,14 +3738,8 @@
       <c r="E59" s="76">
         <v>1E-4</v>
       </c>
-      <c r="F59" s="76">
-        <v>1E-4</v>
-      </c>
-      <c r="G59" s="76">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
         <v>39</v>
       </c>
@@ -4112,14 +3755,8 @@
       <c r="E60" s="76">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="F60" s="76">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="G60" s="76">
-        <v>6.9999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
         <v>40</v>
       </c>
@@ -4135,14 +3772,8 @@
       <c r="E61" s="76">
         <v>1.22E-4</v>
       </c>
-      <c r="F61" s="76">
-        <v>1.22E-4</v>
-      </c>
-      <c r="G61" s="76">
-        <v>1.22E-4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="18" t="s">
         <v>206</v>
       </c>
@@ -4158,14 +3789,8 @@
       <c r="E62" s="76">
         <v>1</v>
       </c>
-      <c r="F62" s="76">
-        <v>1</v>
-      </c>
-      <c r="G62" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="18" t="s">
         <v>41</v>
       </c>
@@ -4181,14 +3806,8 @@
       <c r="E63" s="76">
         <v>0.95</v>
       </c>
-      <c r="F63" s="76">
-        <v>0.95</v>
-      </c>
-      <c r="G63" s="76">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
         <v>407</v>
       </c>
@@ -4204,14 +3823,8 @@
       <c r="E64" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F64" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G64" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="18" t="s">
         <v>90</v>
       </c>
@@ -4227,14 +3840,8 @@
       <c r="E65" s="76">
         <v>5</v>
       </c>
-      <c r="F65" s="76">
-        <v>5</v>
-      </c>
-      <c r="G65" s="76">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="18" t="s">
         <v>409</v>
       </c>
@@ -4250,14 +3857,8 @@
       <c r="E66" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F66" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G66" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
         <v>42</v>
       </c>
@@ -4273,14 +3874,8 @@
       <c r="E67" s="76">
         <v>50</v>
       </c>
-      <c r="F67" s="76">
-        <v>50</v>
-      </c>
-      <c r="G67" s="76">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="18" t="s">
         <v>207</v>
       </c>
@@ -4296,14 +3891,8 @@
       <c r="E68" s="77">
         <v>1453890.8941884842</v>
       </c>
-      <c r="F68" s="77">
-        <v>1453890.8941884842</v>
-      </c>
-      <c r="G68" s="77">
-        <v>1453890.8941884842</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
         <v>43</v>
       </c>
@@ -4319,14 +3908,8 @@
       <c r="E69" s="77">
         <v>1.3888888888888888E-5</v>
       </c>
-      <c r="F69" s="77">
-        <v>1.3888888888888888E-5</v>
-      </c>
-      <c r="G69" s="77">
-        <v>1.3888888888888888E-5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
         <v>44</v>
       </c>
@@ -4342,14 +3925,8 @@
       <c r="E70" s="77">
         <v>6.5011574074074071E-4</v>
       </c>
-      <c r="F70" s="77">
-        <v>6.5011574074074071E-4</v>
-      </c>
-      <c r="G70" s="77">
-        <v>6.5011574074074071E-4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="18" t="s">
         <v>45</v>
       </c>
@@ -4365,14 +3942,8 @@
       <c r="E71" s="76">
         <v>4.7400000000000003E-3</v>
       </c>
-      <c r="F71" s="76">
-        <v>4.7400000000000003E-3</v>
-      </c>
-      <c r="G71" s="76">
-        <v>4.7400000000000003E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="18" t="s">
         <v>46</v>
       </c>
@@ -4388,14 +3959,8 @@
       <c r="E72" s="77">
         <v>282528</v>
       </c>
-      <c r="F72" s="77">
-        <v>282528</v>
-      </c>
-      <c r="G72" s="77">
-        <v>282528</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="18" t="s">
         <v>47</v>
       </c>
@@ -4411,14 +3976,8 @@
       <c r="E73" s="76">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F73" s="76">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G73" s="76">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="18" t="s">
         <v>48</v>
       </c>
@@ -4434,14 +3993,8 @@
       <c r="E74" s="81">
         <v>0.16</v>
       </c>
-      <c r="F74" s="81">
-        <v>0.16</v>
-      </c>
-      <c r="G74" s="81">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="18" t="s">
         <v>49</v>
       </c>
@@ -4457,14 +4010,8 @@
       <c r="E75" s="76">
         <v>0</v>
       </c>
-      <c r="F75" s="76">
-        <v>0</v>
-      </c>
-      <c r="G75" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="34" t="s">
         <v>50</v>
       </c>
@@ -4480,14 +4027,8 @@
       <c r="E76" s="77">
         <v>745476480000</v>
       </c>
-      <c r="F76" s="77">
-        <v>745476480000</v>
-      </c>
-      <c r="G76" s="77">
-        <v>745476480000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="34" t="s">
         <v>204</v>
       </c>
@@ -4503,14 +4044,8 @@
       <c r="E77" s="76">
         <v>100</v>
       </c>
-      <c r="F77" s="76">
-        <v>100</v>
-      </c>
-      <c r="G77" s="76">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="34" t="s">
         <v>415</v>
       </c>
@@ -4526,14 +4061,8 @@
       <c r="E78" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F78" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G78" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="34" t="s">
         <v>400</v>
       </c>
@@ -4549,14 +4078,8 @@
       <c r="E79" s="76">
         <v>21600</v>
       </c>
-      <c r="F79" s="76">
-        <v>21600</v>
-      </c>
-      <c r="G79" s="76">
-        <v>21600</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="34" t="s">
         <v>411</v>
       </c>
@@ -4572,14 +4095,8 @@
       <c r="E80" s="76">
         <v>0.5</v>
       </c>
-      <c r="F80" s="76">
-        <v>0.5</v>
-      </c>
-      <c r="G80" s="76">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="34" t="s">
         <v>401</v>
       </c>
@@ -4595,14 +4112,8 @@
       <c r="E81" s="76">
         <v>60479.999999999993</v>
       </c>
-      <c r="F81" s="76">
-        <v>60479.999999999993</v>
-      </c>
-      <c r="G81" s="76">
-        <v>60479.999999999993</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="34" t="s">
         <v>412</v>
       </c>
@@ -4618,14 +4129,8 @@
       <c r="E82" s="76">
         <v>0.85</v>
       </c>
-      <c r="F82" s="76">
-        <v>0.85</v>
-      </c>
-      <c r="G82" s="76">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="34" t="s">
         <v>402</v>
       </c>
@@ -4641,14 +4146,8 @@
       <c r="E83" s="76">
         <v>518400</v>
       </c>
-      <c r="F83" s="76">
-        <v>518400</v>
-      </c>
-      <c r="G83" s="76">
-        <v>518400</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="34" t="s">
         <v>413</v>
       </c>
@@ -4664,14 +4163,8 @@
       <c r="E84" s="76">
         <v>5184000</v>
       </c>
-      <c r="F84" s="76">
-        <v>5184000</v>
-      </c>
-      <c r="G84" s="76">
-        <v>5184000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="18" t="s">
         <v>51</v>
       </c>
@@ -4687,14 +4180,8 @@
       <c r="E85" s="78">
         <v>50000</v>
       </c>
-      <c r="F85" s="78">
-        <v>50000</v>
-      </c>
-      <c r="G85" s="78">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="18" t="s">
         <v>52</v>
       </c>
@@ -4710,14 +4197,8 @@
       <c r="E86" s="76">
         <v>140000</v>
       </c>
-      <c r="F86" s="76">
-        <v>140000</v>
-      </c>
-      <c r="G86" s="76">
-        <v>140000</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="18" t="s">
         <v>53</v>
       </c>
@@ -4733,14 +4214,8 @@
       <c r="E87" s="77">
         <v>3.6636136999999999E-2</v>
       </c>
-      <c r="F87" s="77">
-        <v>3.6636136999999999E-2</v>
-      </c>
-      <c r="G87" s="77">
-        <v>3.6636136999999999E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
         <v>54</v>
       </c>
@@ -4756,14 +4231,8 @@
       <c r="E88" s="76">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="F88" s="76">
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="G88" s="76">
-        <v>4.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="18" t="s">
         <v>55</v>
       </c>
@@ -4779,14 +4248,8 @@
       <c r="E89" s="76">
         <v>0.05</v>
       </c>
-      <c r="F89" s="76">
-        <v>0.05</v>
-      </c>
-      <c r="G89" s="76">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="18" t="s">
         <v>496</v>
       </c>
@@ -4802,14 +4265,8 @@
       <c r="E90" s="76">
         <v>0</v>
       </c>
-      <c r="F90" s="76">
-        <v>0</v>
-      </c>
-      <c r="G90" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="20" t="s">
         <v>213</v>
       </c>
@@ -4825,14 +4282,8 @@
       <c r="E91" s="76">
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="F91" s="76">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="G91" s="76">
-        <v>6.0000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="20" t="s">
         <v>214</v>
       </c>
@@ -4848,14 +4299,8 @@
       <c r="E92" s="76">
         <v>1E-3</v>
       </c>
-      <c r="F92" s="76">
-        <v>1E-3</v>
-      </c>
-      <c r="G92" s="76">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="20" t="s">
         <v>215</v>
       </c>
@@ -4871,14 +4316,8 @@
       <c r="E93" s="76">
         <v>374999999.99999994</v>
       </c>
-      <c r="F93" s="76">
-        <v>374999999.99999994</v>
-      </c>
-      <c r="G93" s="76">
-        <v>374999999.99999994</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="20" t="s">
         <v>216</v>
       </c>
@@ -4894,14 +4333,8 @@
       <c r="E94" s="77">
         <v>3.7037037037037038E-3</v>
       </c>
-      <c r="F94" s="77">
-        <v>3.7037037037037038E-3</v>
-      </c>
-      <c r="G94" s="77">
-        <v>3.7037037037037038E-3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="20" t="s">
         <v>217</v>
       </c>
@@ -4917,14 +4350,8 @@
       <c r="E95" s="76">
         <v>165600</v>
       </c>
-      <c r="F95" s="76">
-        <v>165600</v>
-      </c>
-      <c r="G95" s="76">
-        <v>165600</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="14" t="s">
         <v>60</v>
       </c>
@@ -4940,14 +4367,8 @@
       <c r="E96" s="76">
         <v>20</v>
       </c>
-      <c r="F96" s="76">
-        <v>20</v>
-      </c>
-      <c r="G96" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="14" t="s">
         <v>208</v>
       </c>
@@ -4963,14 +4384,8 @@
       <c r="E97" s="76">
         <v>1</v>
       </c>
-      <c r="F97" s="76">
-        <v>1</v>
-      </c>
-      <c r="G97" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
         <v>59</v>
       </c>
@@ -4986,14 +4401,8 @@
       <c r="E98" s="76">
         <v>21</v>
       </c>
-      <c r="F98" s="76">
-        <v>21</v>
-      </c>
-      <c r="G98" s="76">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="24" t="s">
         <v>65</v>
       </c>
@@ -5009,14 +4418,8 @@
       <c r="E99" s="76">
         <v>0.64</v>
       </c>
-      <c r="F99" s="76">
-        <v>0.64</v>
-      </c>
-      <c r="G99" s="76">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="24" t="s">
         <v>366</v>
       </c>
@@ -5032,14 +4435,8 @@
       <c r="E100" s="76">
         <v>8</v>
       </c>
-      <c r="F100" s="76">
-        <v>8</v>
-      </c>
-      <c r="G100" s="76">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="24" t="s">
         <v>367</v>
       </c>
@@ -5055,14 +4452,8 @@
       <c r="E101" s="76">
         <v>10</v>
       </c>
-      <c r="F101" s="76">
-        <v>10</v>
-      </c>
-      <c r="G101" s="76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="24" t="s">
         <v>368</v>
       </c>
@@ -5078,14 +4469,8 @@
       <c r="E102" s="76">
         <v>8</v>
       </c>
-      <c r="F102" s="76">
-        <v>8</v>
-      </c>
-      <c r="G102" s="76">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="24" t="s">
         <v>383</v>
       </c>
@@ -5101,14 +4486,8 @@
       <c r="E103" s="76">
         <v>1</v>
       </c>
-      <c r="F103" s="76">
-        <v>1</v>
-      </c>
-      <c r="G103" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="24" t="s">
         <v>385</v>
       </c>
@@ -5124,14 +4503,8 @@
       <c r="E104" s="76">
         <v>0.5</v>
       </c>
-      <c r="F104" s="76">
-        <v>0.5</v>
-      </c>
-      <c r="G104" s="76">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="24" t="s">
         <v>387</v>
       </c>
@@ -5147,14 +4520,8 @@
       <c r="E105" s="76">
         <v>0</v>
       </c>
-      <c r="F105" s="76">
-        <v>0</v>
-      </c>
-      <c r="G105" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="24" t="s">
         <v>389</v>
       </c>
@@ -5170,14 +4537,8 @@
       <c r="E106" s="82">
         <v>1589759.9999999998</v>
       </c>
-      <c r="F106" s="82">
-        <v>1589759.9999999998</v>
-      </c>
-      <c r="G106" s="82">
-        <v>1589759.9999999998</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="24" t="s">
         <v>391</v>
       </c>
@@ -5193,14 +4554,8 @@
       <c r="E107" s="82">
         <v>455327.99999999994</v>
       </c>
-      <c r="F107" s="82">
-        <v>455327.99999999994</v>
-      </c>
-      <c r="G107" s="82">
-        <v>455327.99999999994</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="24" t="s">
         <v>393</v>
       </c>
@@ -5216,14 +4571,8 @@
       <c r="E108" s="82">
         <v>664416</v>
       </c>
-      <c r="F108" s="82">
-        <v>664416</v>
-      </c>
-      <c r="G108" s="82">
-        <v>664416</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="24" t="s">
         <v>422</v>
       </c>
@@ -5239,14 +4588,8 @@
       <c r="E109" s="82">
         <v>100</v>
       </c>
-      <c r="F109" s="82">
-        <v>100</v>
-      </c>
-      <c r="G109" s="82">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="24" t="s">
         <v>424</v>
       </c>
@@ -5262,14 +4605,8 @@
       <c r="E110" s="82">
         <v>280800</v>
       </c>
-      <c r="F110" s="82">
-        <v>280800</v>
-      </c>
-      <c r="G110" s="82">
-        <v>280800</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="24" t="s">
         <v>426</v>
       </c>
@@ -5285,14 +4622,8 @@
       <c r="E111" s="83">
         <v>1.2847222222222224E-5</v>
       </c>
-      <c r="F111" s="83">
-        <v>1.2847222222222224E-5</v>
-      </c>
-      <c r="G111" s="83">
-        <v>1.2847222222222224E-5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="24" t="s">
         <v>428</v>
       </c>
@@ -5308,14 +4639,8 @@
       <c r="E112" s="82">
         <v>90</v>
       </c>
-      <c r="F112" s="82">
-        <v>90</v>
-      </c>
-      <c r="G112" s="82">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="24" t="s">
         <v>430</v>
       </c>
@@ -5331,14 +4656,8 @@
       <c r="E113" s="82">
         <v>459648</v>
       </c>
-      <c r="F113" s="82">
-        <v>459648</v>
-      </c>
-      <c r="G113" s="82">
-        <v>459648</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="24" t="s">
         <v>432</v>
       </c>
@@ -5354,14 +4673,8 @@
       <c r="E114" s="83">
         <v>1.2847222222222224E-5</v>
       </c>
-      <c r="F114" s="83">
-        <v>1.2847222222222224E-5</v>
-      </c>
-      <c r="G114" s="83">
-        <v>1.2847222222222224E-5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="24" t="s">
         <v>395</v>
       </c>
@@ -5377,14 +4690,8 @@
       <c r="E115" s="82">
         <v>21600</v>
       </c>
-      <c r="F115" s="82">
-        <v>21600</v>
-      </c>
-      <c r="G115" s="82">
-        <v>21600</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
         <v>397</v>
       </c>
@@ -5400,14 +4707,8 @@
       <c r="E116" s="82">
         <v>43200</v>
       </c>
-      <c r="F116" s="82">
-        <v>43200</v>
-      </c>
-      <c r="G116" s="82">
-        <v>43200</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="14" t="s">
         <v>61</v>
       </c>
@@ -5423,14 +4724,8 @@
       <c r="E117" s="76">
         <v>0.8</v>
       </c>
-      <c r="F117" s="76">
-        <v>0.8</v>
-      </c>
-      <c r="G117" s="76">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="14" t="s">
         <v>62</v>
       </c>
@@ -5446,14 +4741,8 @@
       <c r="E118" s="77">
         <v>2.0833333333333335E-4</v>
       </c>
-      <c r="F118" s="77">
-        <v>2.0833333333333335E-4</v>
-      </c>
-      <c r="G118" s="77">
-        <v>2.0833333333333335E-4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="14" t="s">
         <v>63</v>
       </c>
@@ -5469,14 +4758,8 @@
       <c r="E119" s="83">
         <v>5.7899999999999998E-7</v>
       </c>
-      <c r="F119" s="83">
-        <v>5.7899999999999998E-7</v>
-      </c>
-      <c r="G119" s="83">
-        <v>5.7899999999999998E-7</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="14" t="s">
         <v>64</v>
       </c>
@@ -5492,14 +4775,8 @@
       <c r="E120" s="77">
         <v>2.0833333333333335E-4</v>
       </c>
-      <c r="F120" s="77">
-        <v>2.0833333333333335E-4</v>
-      </c>
-      <c r="G120" s="77">
-        <v>2.0833333333333335E-4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="14" t="s">
         <v>463</v>
       </c>
@@ -5515,14 +4792,8 @@
       <c r="E121" s="77">
         <v>0</v>
       </c>
-      <c r="F121" s="77">
-        <v>0</v>
-      </c>
-      <c r="G121" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="14" t="s">
         <v>464</v>
       </c>
@@ -5538,14 +4809,8 @@
       <c r="E122" s="77">
         <v>0</v>
       </c>
-      <c r="F122" s="77">
-        <v>0</v>
-      </c>
-      <c r="G122" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="22" t="s">
         <v>445</v>
       </c>
@@ -5561,14 +4826,8 @@
       <c r="E123" s="84" t="s">
         <v>406</v>
       </c>
-      <c r="F123" s="84" t="s">
-        <v>406</v>
-      </c>
-      <c r="G123" s="84" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="22" t="s">
         <v>67</v>
       </c>
@@ -5584,14 +4843,8 @@
       <c r="E124" s="84" t="s">
         <v>406</v>
       </c>
-      <c r="F124" s="84" t="s">
-        <v>406</v>
-      </c>
-      <c r="G124" s="84" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="22" t="s">
         <v>459</v>
       </c>
@@ -5607,14 +4860,8 @@
       <c r="E125" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="F125" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="G125" s="84" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="22" t="s">
         <v>66</v>
       </c>
@@ -5630,14 +4877,8 @@
       <c r="E126" s="78">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F126" s="78">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="G126" s="78">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="22" t="s">
         <v>441</v>
       </c>
@@ -5653,14 +4894,8 @@
       <c r="E127" s="78">
         <v>4.9999999999999999E-13</v>
       </c>
-      <c r="F127" s="78">
-        <v>4.9999999999999999E-13</v>
-      </c>
-      <c r="G127" s="78">
-        <v>4.9999999999999999E-13</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
         <v>450</v>
       </c>
@@ -5676,14 +4911,8 @@
       <c r="E128" s="76">
         <v>10</v>
       </c>
-      <c r="F128" s="76">
-        <v>10</v>
-      </c>
-      <c r="G128" s="76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="22" t="s">
         <v>451</v>
       </c>
@@ -5699,14 +4928,8 @@
       <c r="E129" s="76">
         <v>-0.04</v>
       </c>
-      <c r="F129" s="76">
-        <v>-0.04</v>
-      </c>
-      <c r="G129" s="76">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="22" t="s">
         <v>452</v>
       </c>
@@ -5722,14 +4945,8 @@
       <c r="E130" s="76">
         <v>2.9</v>
       </c>
-      <c r="F130" s="76">
-        <v>2.9</v>
-      </c>
-      <c r="G130" s="76">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="22" t="s">
         <v>453</v>
       </c>
@@ -5745,14 +4962,8 @@
       <c r="E131" s="76">
         <v>1</v>
       </c>
-      <c r="F131" s="76">
-        <v>1</v>
-      </c>
-      <c r="G131" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="22" t="s">
         <v>444</v>
       </c>
@@ -5768,14 +4979,8 @@
       <c r="E132" s="78">
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="F132" s="78">
-        <v>1.9999999999999999E-7</v>
-      </c>
-      <c r="G132" s="78">
-        <v>1.9999999999999999E-7</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="22" t="s">
         <v>232</v>
       </c>
@@ -5791,14 +4996,8 @@
       <c r="E133" s="76">
         <v>10</v>
       </c>
-      <c r="F133" s="76">
-        <v>10</v>
-      </c>
-      <c r="G133" s="76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
         <v>233</v>
       </c>
@@ -5814,14 +5013,8 @@
       <c r="E134" s="76">
         <v>-0.04</v>
       </c>
-      <c r="F134" s="76">
-        <v>-0.04</v>
-      </c>
-      <c r="G134" s="76">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="22" t="s">
         <v>234</v>
       </c>
@@ -5837,14 +5030,8 @@
       <c r="E135" s="76">
         <v>2.9</v>
       </c>
-      <c r="F135" s="76">
-        <v>2.9</v>
-      </c>
-      <c r="G135" s="76">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="22" t="s">
         <v>235</v>
       </c>
@@ -5860,14 +5047,8 @@
       <c r="E136" s="76">
         <v>1</v>
       </c>
-      <c r="F136" s="76">
-        <v>1</v>
-      </c>
-      <c r="G136" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="22" t="s">
         <v>69</v>
       </c>
@@ -5883,14 +5064,8 @@
       <c r="E137" s="76">
         <v>0</v>
       </c>
-      <c r="F137" s="76">
-        <v>0</v>
-      </c>
-      <c r="G137" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="22" t="s">
         <v>70</v>
       </c>
@@ -5906,14 +5081,8 @@
       <c r="E138" s="78">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="F138" s="78">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="G138" s="78">
-        <v>5.0000000000000004E-6</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="24" t="s">
         <v>56</v>
       </c>
@@ -5929,14 +5098,8 @@
       <c r="E139" s="76">
         <v>0</v>
       </c>
-      <c r="F139" s="76">
-        <v>0</v>
-      </c>
-      <c r="G139" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="24" t="s">
         <v>57</v>
       </c>
@@ -5952,14 +5115,8 @@
       <c r="E140" s="76">
         <v>2E-3</v>
       </c>
-      <c r="F140" s="76">
-        <v>2E-3</v>
-      </c>
-      <c r="G140" s="76">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="24" t="s">
         <v>58</v>
       </c>
@@ -5975,14 +5132,8 @@
       <c r="E141" s="78">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="F141" s="78">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="G141" s="78">
-        <v>3.9999999999999998E-6</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="24" t="s">
         <v>71</v>
       </c>
@@ -5998,14 +5149,8 @@
       <c r="E142" s="78">
         <v>3.7699999999999999E-10</v>
       </c>
-      <c r="F142" s="78">
-        <v>3.7699999999999999E-10</v>
-      </c>
-      <c r="G142" s="78">
-        <v>3.7699999999999999E-10</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="24" t="s">
         <v>236</v>
       </c>
@@ -6021,14 +5166,8 @@
       <c r="E143" s="76">
         <v>20</v>
       </c>
-      <c r="F143" s="76">
-        <v>20</v>
-      </c>
-      <c r="G143" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="24" t="s">
         <v>237</v>
       </c>
@@ -6044,14 +5183,8 @@
       <c r="E144" s="76">
         <v>-0.06</v>
       </c>
-      <c r="F144" s="76">
-        <v>-0.06</v>
-      </c>
-      <c r="G144" s="76">
-        <v>-0.06</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
         <v>238</v>
       </c>
@@ -6067,14 +5200,8 @@
       <c r="E145" s="76">
         <v>0.89100000000000001</v>
       </c>
-      <c r="F145" s="76">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="G145" s="76">
-        <v>0.89100000000000001</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
         <v>239</v>
       </c>
@@ -6090,14 +5217,8 @@
       <c r="E146" s="76">
         <v>1</v>
       </c>
-      <c r="F146" s="76">
-        <v>1</v>
-      </c>
-      <c r="G146" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="24" t="s">
         <v>72</v>
       </c>
@@ -6113,14 +5234,8 @@
       <c r="E147" s="78">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="F147" s="78">
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="G147" s="78">
-        <v>4.0000000000000003E-5</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
         <v>73</v>
       </c>
@@ -6136,14 +5251,8 @@
       <c r="E148" s="78">
         <v>5.8333333333333335E-9</v>
       </c>
-      <c r="F148" s="78">
-        <v>5.8333333333333335E-9</v>
-      </c>
-      <c r="G148" s="78">
-        <v>5.8333333333333335E-9</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="14" t="s">
         <v>240</v>
       </c>
@@ -6159,14 +5268,8 @@
       <c r="E149" s="76">
         <v>20</v>
       </c>
-      <c r="F149" s="76">
-        <v>20</v>
-      </c>
-      <c r="G149" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
         <v>241</v>
       </c>
@@ -6182,14 +5285,8 @@
       <c r="E150" s="76">
         <v>-0.06</v>
       </c>
-      <c r="F150" s="76">
-        <v>-0.06</v>
-      </c>
-      <c r="G150" s="76">
-        <v>-0.06</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="14" t="s">
         <v>242</v>
       </c>
@@ -6205,14 +5302,8 @@
       <c r="E151" s="76">
         <v>0.89100000000000001</v>
       </c>
-      <c r="F151" s="76">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="G151" s="76">
-        <v>0.89100000000000001</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="14" t="s">
         <v>243</v>
       </c>
@@ -6228,14 +5319,8 @@
       <c r="E152" s="76">
         <v>1</v>
       </c>
-      <c r="F152" s="76">
-        <v>1</v>
-      </c>
-      <c r="G152" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="14" t="s">
         <v>74</v>
       </c>
@@ -6251,14 +5336,8 @@
       <c r="E153" s="78">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="F153" s="78">
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="G153" s="78">
-        <v>4.0000000000000003E-5</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="10" t="s">
         <v>75</v>
       </c>
@@ -6274,14 +5353,8 @@
       <c r="E154" s="78">
         <v>4.0000000000000001E-8</v>
       </c>
-      <c r="F154" s="78">
-        <v>4.0000000000000001E-8</v>
-      </c>
-      <c r="G154" s="78">
-        <v>4.0000000000000001E-8</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="10" t="s">
         <v>218</v>
       </c>
@@ -6297,14 +5370,8 @@
       <c r="E155" s="76">
         <v>20</v>
       </c>
-      <c r="F155" s="76">
-        <v>20</v>
-      </c>
-      <c r="G155" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="10" t="s">
         <v>219</v>
       </c>
@@ -6320,14 +5387,8 @@
       <c r="E156" s="76">
         <v>-4.4200000000000003E-2</v>
       </c>
-      <c r="F156" s="76">
-        <v>-4.4200000000000003E-2</v>
-      </c>
-      <c r="G156" s="76">
-        <v>-4.4200000000000003E-2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="10" t="s">
         <v>220</v>
       </c>
@@ -6343,14 +5404,8 @@
       <c r="E157" s="76">
         <v>1.55</v>
       </c>
-      <c r="F157" s="76">
-        <v>1.55</v>
-      </c>
-      <c r="G157" s="76">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="10" t="s">
         <v>221</v>
       </c>
@@ -6366,14 +5421,8 @@
       <c r="E158" s="76">
         <v>1</v>
       </c>
-      <c r="F158" s="76">
-        <v>1</v>
-      </c>
-      <c r="G158" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="10" t="s">
         <v>76</v>
       </c>
@@ -6389,14 +5438,8 @@
       <c r="E159" s="76">
         <v>2.7799999999999998E-4</v>
       </c>
-      <c r="F159" s="76">
-        <v>2.7799999999999998E-4</v>
-      </c>
-      <c r="G159" s="76">
-        <v>2.7799999999999998E-4</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="26" t="s">
         <v>78</v>
       </c>
@@ -6412,14 +5455,8 @@
       <c r="E160" s="78">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="F160" s="78">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="G160" s="78">
-        <v>2.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="26" t="s">
         <v>245</v>
       </c>
@@ -6435,14 +5472,8 @@
       <c r="E161" s="76">
         <v>20</v>
       </c>
-      <c r="F161" s="76">
-        <v>20</v>
-      </c>
-      <c r="G161" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="26" t="s">
         <v>246</v>
       </c>
@@ -6458,14 +5489,8 @@
       <c r="E162" s="76">
         <v>0</v>
       </c>
-      <c r="F162" s="76">
-        <v>0</v>
-      </c>
-      <c r="G162" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="26" t="s">
         <v>247</v>
       </c>
@@ -6481,14 +5506,8 @@
       <c r="E163" s="76">
         <v>1</v>
       </c>
-      <c r="F163" s="76">
-        <v>1</v>
-      </c>
-      <c r="G163" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="26" t="s">
         <v>248</v>
       </c>
@@ -6504,14 +5523,8 @@
       <c r="E164" s="76">
         <v>0</v>
       </c>
-      <c r="F164" s="76">
-        <v>0</v>
-      </c>
-      <c r="G164" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="26" t="s">
         <v>79</v>
       </c>
@@ -6527,14 +5540,8 @@
       <c r="E165" s="76">
         <v>0.4</v>
       </c>
-      <c r="F165" s="76">
-        <v>0.4</v>
-      </c>
-      <c r="G165" s="76">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="32" t="s">
         <v>80</v>
       </c>
@@ -6550,14 +5557,8 @@
       <c r="E166" s="78">
         <v>2.0000000000000001E-9</v>
       </c>
-      <c r="F166" s="78">
-        <v>2.0000000000000001E-9</v>
-      </c>
-      <c r="G166" s="78">
-        <v>2.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="32" t="s">
         <v>249</v>
       </c>
@@ -6573,14 +5574,8 @@
       <c r="E167" s="76">
         <v>25</v>
       </c>
-      <c r="F167" s="76">
-        <v>25</v>
-      </c>
-      <c r="G167" s="76">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="32" t="s">
         <v>250</v>
       </c>
@@ -6596,14 +5591,8 @@
       <c r="E168" s="76">
         <v>0</v>
       </c>
-      <c r="F168" s="76">
-        <v>0</v>
-      </c>
-      <c r="G168" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="32" t="s">
         <v>251</v>
       </c>
@@ -6619,14 +5608,8 @@
       <c r="E169" s="76">
         <v>3.98</v>
       </c>
-      <c r="F169" s="76">
-        <v>3.98</v>
-      </c>
-      <c r="G169" s="76">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="32" t="s">
         <v>252</v>
       </c>
@@ -6642,14 +5625,8 @@
       <c r="E170" s="76">
         <v>1</v>
       </c>
-      <c r="F170" s="76">
-        <v>1</v>
-      </c>
-      <c r="G170" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="32" t="s">
         <v>81</v>
       </c>
@@ -6665,14 +5642,8 @@
       <c r="E171" s="77">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="F171" s="77">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="G171" s="77">
-        <v>5.0000000000000004E-6</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
         <v>253</v>
       </c>
@@ -6688,14 +5659,8 @@
       <c r="E172" s="78">
         <v>1E-8</v>
       </c>
-      <c r="F172" s="78">
-        <v>1E-8</v>
-      </c>
-      <c r="G172" s="78">
-        <v>1E-8</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="12" t="s">
         <v>254</v>
       </c>
@@ -6711,14 +5676,8 @@
       <c r="E173" s="76">
         <v>20</v>
       </c>
-      <c r="F173" s="76">
-        <v>20</v>
-      </c>
-      <c r="G173" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
         <v>255</v>
       </c>
@@ -6734,14 +5693,8 @@
       <c r="E174" s="76">
         <v>0</v>
       </c>
-      <c r="F174" s="76">
-        <v>0</v>
-      </c>
-      <c r="G174" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
         <v>256</v>
       </c>
@@ -6757,14 +5710,8 @@
       <c r="E175" s="76">
         <v>2</v>
       </c>
-      <c r="F175" s="76">
-        <v>2</v>
-      </c>
-      <c r="G175" s="76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
         <v>257</v>
       </c>
@@ -6780,14 +5727,8 @@
       <c r="E176" s="76">
         <v>1</v>
       </c>
-      <c r="F176" s="76">
-        <v>1</v>
-      </c>
-      <c r="G176" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="12" t="s">
         <v>258</v>
       </c>
@@ -6803,14 +5744,8 @@
       <c r="E177" s="77">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="F177" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-      <c r="G177" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
         <v>259</v>
       </c>
@@ -6826,14 +5761,8 @@
       <c r="E178" s="76">
         <v>1</v>
       </c>
-      <c r="F178" s="76">
-        <v>1</v>
-      </c>
-      <c r="G178" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="28" t="s">
         <v>260</v>
       </c>
@@ -6849,14 +5778,8 @@
       <c r="E179" s="76">
         <v>2.3533050791148899E-8</v>
       </c>
-      <c r="F179" s="76">
-        <v>2.3533050791148899E-8</v>
-      </c>
-      <c r="G179" s="76">
-        <v>2.3533050791148899E-8</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="28" t="s">
         <v>261</v>
       </c>
@@ -6872,14 +5795,8 @@
       <c r="E180" s="76">
         <v>20</v>
       </c>
-      <c r="F180" s="76">
-        <v>20</v>
-      </c>
-      <c r="G180" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="28" t="s">
         <v>262</v>
       </c>
@@ -6895,14 +5812,8 @@
       <c r="E181" s="76">
         <v>-0.187</v>
       </c>
-      <c r="F181" s="76">
-        <v>-0.187</v>
-      </c>
-      <c r="G181" s="76">
-        <v>-0.187</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="28" t="s">
         <v>263</v>
       </c>
@@ -6918,14 +5829,8 @@
       <c r="E182" s="76">
         <v>2.48</v>
       </c>
-      <c r="F182" s="76">
-        <v>2.48</v>
-      </c>
-      <c r="G182" s="76">
-        <v>2.48</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="28" t="s">
         <v>264</v>
       </c>
@@ -6941,14 +5846,8 @@
       <c r="E183" s="76">
         <v>1</v>
       </c>
-      <c r="F183" s="76">
-        <v>1</v>
-      </c>
-      <c r="G183" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="28" t="s">
         <v>265</v>
       </c>
@@ -6964,14 +5863,8 @@
       <c r="E184" s="76">
         <v>6.1060227588121015E-4</v>
       </c>
-      <c r="F184" s="76">
-        <v>6.1060227588121015E-4</v>
-      </c>
-      <c r="G184" s="76">
-        <v>6.1060227588121015E-4</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="24" t="s">
         <v>266</v>
       </c>
@@ -6987,14 +5880,8 @@
       <c r="E185" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-      <c r="F185" s="85">
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="G185" s="85">
-        <v>3.9999999999999998E-7</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="24" t="s">
         <v>267</v>
       </c>
@@ -7010,14 +5897,8 @@
       <c r="E186" s="85">
         <v>25</v>
       </c>
-      <c r="F186" s="85">
-        <v>25</v>
-      </c>
-      <c r="G186" s="85">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="24" t="s">
         <v>268</v>
       </c>
@@ -7033,14 +5914,8 @@
       <c r="E187" s="85">
         <v>0</v>
       </c>
-      <c r="F187" s="85">
-        <v>0</v>
-      </c>
-      <c r="G187" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="24" t="s">
         <v>269</v>
       </c>
@@ -7056,14 +5931,8 @@
       <c r="E188" s="85">
         <v>3.98</v>
       </c>
-      <c r="F188" s="85">
-        <v>3.98</v>
-      </c>
-      <c r="G188" s="85">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="24" t="s">
         <v>270</v>
       </c>
@@ -7079,14 +5948,8 @@
       <c r="E189" s="85">
         <v>1</v>
       </c>
-      <c r="F189" s="85">
-        <v>1</v>
-      </c>
-      <c r="G189" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="24" t="s">
         <v>271</v>
       </c>
@@ -7102,14 +5965,8 @@
       <c r="E190" s="77">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="F190" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-      <c r="G190" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="8" t="s">
         <v>272</v>
       </c>
@@ -7125,14 +5982,8 @@
       <c r="E191" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-      <c r="F191" s="85">
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="G191" s="85">
-        <v>3.9999999999999998E-7</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="8" t="s">
         <v>273</v>
       </c>
@@ -7148,14 +5999,8 @@
       <c r="E192" s="85">
         <v>25</v>
       </c>
-      <c r="F192" s="85">
-        <v>25</v>
-      </c>
-      <c r="G192" s="85">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="8" t="s">
         <v>274</v>
       </c>
@@ -7171,14 +6016,8 @@
       <c r="E193" s="85">
         <v>0</v>
       </c>
-      <c r="F193" s="85">
-        <v>0</v>
-      </c>
-      <c r="G193" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="8" t="s">
         <v>275</v>
       </c>
@@ -7194,14 +6033,8 @@
       <c r="E194" s="85">
         <v>3.98</v>
       </c>
-      <c r="F194" s="85">
-        <v>3.98</v>
-      </c>
-      <c r="G194" s="85">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="8" t="s">
         <v>276</v>
       </c>
@@ -7217,14 +6050,8 @@
       <c r="E195" s="85">
         <v>1</v>
       </c>
-      <c r="F195" s="85">
-        <v>1</v>
-      </c>
-      <c r="G195" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="8" t="s">
         <v>277</v>
       </c>
@@ -7240,14 +6067,8 @@
       <c r="E196" s="77">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="F196" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-      <c r="G196" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="30" t="s">
         <v>278</v>
       </c>
@@ -7263,14 +6084,8 @@
       <c r="E197" s="85">
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="F197" s="85">
-        <v>1.9999999999999999E-7</v>
-      </c>
-      <c r="G197" s="85">
-        <v>1.9999999999999999E-7</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="30" t="s">
         <v>279</v>
       </c>
@@ -7286,14 +6101,8 @@
       <c r="E198" s="85">
         <v>25</v>
       </c>
-      <c r="F198" s="85">
-        <v>25</v>
-      </c>
-      <c r="G198" s="85">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="30" t="s">
         <v>280</v>
       </c>
@@ -7309,14 +6118,8 @@
       <c r="E199" s="85">
         <v>0</v>
       </c>
-      <c r="F199" s="85">
-        <v>0</v>
-      </c>
-      <c r="G199" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="30" t="s">
         <v>281</v>
       </c>
@@ -7332,14 +6135,8 @@
       <c r="E200" s="85">
         <v>3.98</v>
       </c>
-      <c r="F200" s="85">
-        <v>3.98</v>
-      </c>
-      <c r="G200" s="85">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="30" t="s">
         <v>282</v>
       </c>
@@ -7355,14 +6152,8 @@
       <c r="E201" s="85">
         <v>1</v>
       </c>
-      <c r="F201" s="85">
-        <v>1</v>
-      </c>
-      <c r="G201" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="30" t="s">
         <v>283</v>
       </c>
@@ -7378,14 +6169,8 @@
       <c r="E202" s="77">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="F202" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-      <c r="G202" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="73" t="s">
         <v>361</v>
       </c>
@@ -7401,17 +6186,9 @@
       <c r="E203" s="86" t="s">
         <v>482</v>
       </c>
-      <c r="F203" s="86" t="s">
-        <v>482</v>
-      </c>
-      <c r="G203" s="86" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E204" s="38"/>
-      <c r="F204" s="38"/>
-      <c r="G204" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
After refining the input reading
</commit_message>
<xml_diff>
--- a/tutorial/inputs/scenarios_list.xlsx
+++ b/tutorial/inputs/scenarios_list.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="501">
   <si>
     <t>input_file</t>
   </si>
@@ -2162,7 +2162,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2342,9 +2342,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="51" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="52" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="52" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2721,13 +2718,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G204"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B177" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G193" sqref="G193"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2736,10 +2733,10 @@
     <col min="2" max="2" width="64.77734375" customWidth="1"/>
     <col min="3" max="3" width="19.88671875" customWidth="1"/>
     <col min="4" max="4" width="17" style="38" customWidth="1"/>
-    <col min="5" max="7" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>94</v>
       </c>
@@ -2755,14 +2752,8 @@
       <c r="E1" s="87">
         <v>208</v>
       </c>
-      <c r="F1" s="87">
-        <v>209</v>
-      </c>
-      <c r="G1" s="87">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2778,14 +2769,8 @@
       <c r="E2" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2801,14 +2786,8 @@
       <c r="E3" s="76">
         <v>1</v>
       </c>
-      <c r="F3" s="76">
-        <v>1</v>
-      </c>
-      <c r="G3" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
         <v>454</v>
       </c>
@@ -2824,14 +2803,8 @@
       <c r="E4" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="70" t="s">
         <v>455</v>
       </c>
@@ -2847,14 +2820,8 @@
       <c r="E5" s="76" t="s">
         <v>458</v>
       </c>
-      <c r="F5" s="76" t="s">
-        <v>458</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -2870,14 +2837,8 @@
       <c r="E6" s="76">
         <v>180</v>
       </c>
-      <c r="F6" s="76">
-        <v>180</v>
-      </c>
-      <c r="G6" s="76">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -2893,14 +2854,8 @@
       <c r="E7" s="77">
         <v>4.1666666999999998E-2</v>
       </c>
-      <c r="F7" s="77">
-        <v>4.1666666999999998E-2</v>
-      </c>
-      <c r="G7" s="77">
-        <v>4.1666666999999998E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>20</v>
       </c>
@@ -2916,14 +2871,8 @@
       <c r="E8" s="77">
         <v>4.1666666999999998E-2</v>
       </c>
-      <c r="F8" s="88">
-        <v>1</v>
-      </c>
-      <c r="G8" s="88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
@@ -2936,17 +2885,11 @@
       <c r="D9" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="89" t="s">
+      <c r="E9" s="88" t="s">
         <v>498</v>
       </c>
-      <c r="F9" s="76" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="76" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
@@ -2962,14 +2905,8 @@
       <c r="E10" s="76">
         <v>1</v>
       </c>
-      <c r="F10" s="76">
-        <v>1</v>
-      </c>
-      <c r="G10" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>461</v>
       </c>
@@ -2985,14 +2922,8 @@
       <c r="E11" s="76">
         <v>0</v>
       </c>
-      <c r="F11" s="76">
-        <v>0</v>
-      </c>
-      <c r="G11" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>6</v>
       </c>
@@ -3008,14 +2939,8 @@
       <c r="E12" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -3031,14 +2956,8 @@
       <c r="E13" s="78">
         <v>5.0000000000000001E-9</v>
       </c>
-      <c r="F13" s="78">
-        <v>5.0000000000000001E-9</v>
-      </c>
-      <c r="G13" s="78">
-        <v>5.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
@@ -3054,14 +2973,8 @@
       <c r="E14" s="76">
         <v>10</v>
       </c>
-      <c r="F14" s="76">
-        <v>10</v>
-      </c>
-      <c r="G14" s="76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>479</v>
       </c>
@@ -3077,14 +2990,8 @@
       <c r="E15" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="89" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>480</v>
       </c>
@@ -3100,14 +3007,8 @@
       <c r="E16" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>483</v>
       </c>
@@ -3123,14 +3024,8 @@
       <c r="E17" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G17" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>499</v>
       </c>
@@ -3146,14 +3041,8 @@
       <c r="E18" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" s="89" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>484</v>
       </c>
@@ -3169,14 +3058,8 @@
       <c r="E19" s="76">
         <v>86400</v>
       </c>
-      <c r="F19" s="76">
-        <v>86400</v>
-      </c>
-      <c r="G19" s="76">
-        <v>86400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>10</v>
       </c>
@@ -3192,14 +3075,8 @@
       <c r="E20" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>11</v>
       </c>
@@ -3215,14 +3092,8 @@
       <c r="E21" s="76">
         <v>3</v>
       </c>
-      <c r="F21" s="76">
-        <v>3</v>
-      </c>
-      <c r="G21" s="76">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>362</v>
       </c>
@@ -3238,14 +3109,8 @@
       <c r="E22" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="79" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>364</v>
       </c>
@@ -3261,14 +3126,8 @@
       <c r="E23" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F23" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" s="79" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>376</v>
       </c>
@@ -3284,14 +3143,8 @@
       <c r="E24" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>375</v>
       </c>
@@ -3307,14 +3160,8 @@
       <c r="E25" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G25" s="79" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>374</v>
       </c>
@@ -3330,14 +3177,8 @@
       <c r="E26" s="79" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G26" s="79" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>12</v>
       </c>
@@ -3353,14 +3194,8 @@
       <c r="E27" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>13</v>
       </c>
@@ -3376,14 +3211,8 @@
       <c r="E28" s="76">
         <v>0.33</v>
       </c>
-      <c r="F28" s="76">
-        <v>0.33</v>
-      </c>
-      <c r="G28" s="76">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>14</v>
       </c>
@@ -3399,14 +3228,8 @@
       <c r="E29" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>9</v>
       </c>
@@ -3422,14 +3245,8 @@
       <c r="E30" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F30" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G30" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>467</v>
       </c>
@@ -3445,14 +3262,8 @@
       <c r="E31" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F31" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
         <v>21</v>
       </c>
@@ -3468,14 +3279,8 @@
       <c r="E32" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F32" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G32" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
         <v>22</v>
       </c>
@@ -3491,14 +3296,8 @@
       <c r="E33" s="76" t="s">
         <v>487</v>
       </c>
-      <c r="F33" s="76" t="s">
-        <v>487</v>
-      </c>
-      <c r="G33" s="76" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>23</v>
       </c>
@@ -3514,14 +3313,8 @@
       <c r="E34" s="78">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F34" s="78">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G34" s="78">
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
         <v>24</v>
       </c>
@@ -3537,14 +3330,8 @@
       <c r="E35" s="78">
         <v>1E-3</v>
       </c>
-      <c r="F35" s="78">
-        <v>1E-3</v>
-      </c>
-      <c r="G35" s="78">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
         <v>25</v>
       </c>
@@ -3560,14 +3347,8 @@
       <c r="E36" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F36" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G36" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
         <v>26</v>
       </c>
@@ -3583,14 +3364,8 @@
       <c r="E37" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="F37" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="G37" s="76" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
         <v>27</v>
       </c>
@@ -3606,14 +3381,8 @@
       <c r="E38" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F38" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G38" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="14" t="s">
         <v>28</v>
       </c>
@@ -3629,14 +3398,8 @@
       <c r="E39" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F39" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G39" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
         <v>29</v>
       </c>
@@ -3652,14 +3415,8 @@
       <c r="E40" s="76">
         <v>120</v>
       </c>
-      <c r="F40" s="76">
-        <v>120</v>
-      </c>
-      <c r="G40" s="76">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="14" t="s">
         <v>30</v>
       </c>
@@ -3675,14 +3432,8 @@
       <c r="E41" s="76">
         <v>0</v>
       </c>
-      <c r="F41" s="76">
-        <v>0</v>
-      </c>
-      <c r="G41" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
         <v>31</v>
       </c>
@@ -3698,14 +3449,8 @@
       <c r="E42" s="76">
         <v>0</v>
       </c>
-      <c r="F42" s="76">
-        <v>0</v>
-      </c>
-      <c r="G42" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
         <v>32</v>
       </c>
@@ -3721,14 +3466,8 @@
       <c r="E43" s="76">
         <v>-0.1</v>
       </c>
-      <c r="F43" s="76">
-        <v>-0.1</v>
-      </c>
-      <c r="G43" s="76">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="14" t="s">
         <v>476</v>
       </c>
@@ -3744,14 +3483,8 @@
       <c r="E44" s="76">
         <v>-0.2</v>
       </c>
-      <c r="F44" s="76">
-        <v>-0.2</v>
-      </c>
-      <c r="G44" s="76">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="14" t="s">
         <v>477</v>
       </c>
@@ -3767,14 +3500,8 @@
       <c r="E45" s="76">
         <v>-0.2</v>
       </c>
-      <c r="F45" s="76">
-        <v>-0.2</v>
-      </c>
-      <c r="G45" s="76">
-        <v>-0.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
         <v>33</v>
       </c>
@@ -3790,14 +3517,8 @@
       <c r="E46" s="76">
         <v>0.4</v>
       </c>
-      <c r="F46" s="76">
-        <v>0.4</v>
-      </c>
-      <c r="G46" s="76">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="14" t="s">
         <v>35</v>
       </c>
@@ -3813,14 +3534,8 @@
       <c r="E47" s="76">
         <v>0</v>
       </c>
-      <c r="F47" s="76">
-        <v>0</v>
-      </c>
-      <c r="G47" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="14" t="s">
         <v>437</v>
       </c>
@@ -3836,14 +3551,8 @@
       <c r="E48" s="76">
         <v>1200</v>
       </c>
-      <c r="F48" s="76">
-        <v>1200</v>
-      </c>
-      <c r="G48" s="76">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="14" t="s">
         <v>438</v>
       </c>
@@ -3859,14 +3568,8 @@
       <c r="E49" s="76">
         <v>1200</v>
       </c>
-      <c r="F49" s="76">
-        <v>1200</v>
-      </c>
-      <c r="G49" s="76">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="14" t="s">
         <v>470</v>
       </c>
@@ -3882,14 +3585,8 @@
       <c r="E50" s="80" t="s">
         <v>472</v>
       </c>
-      <c r="F50" s="80" t="s">
-        <v>472</v>
-      </c>
-      <c r="G50" s="80" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="14" t="s">
         <v>15</v>
       </c>
@@ -3905,14 +3602,8 @@
       <c r="E51" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F51" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G51" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>16</v>
       </c>
@@ -3928,14 +3619,8 @@
       <c r="E52" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F52" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G52" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>17</v>
       </c>
@@ -3951,14 +3636,8 @@
       <c r="E53" s="76">
         <v>0</v>
       </c>
-      <c r="F53" s="76">
-        <v>0</v>
-      </c>
-      <c r="G53" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>18</v>
       </c>
@@ -3974,14 +3653,8 @@
       <c r="E54" s="76">
         <v>0.5</v>
       </c>
-      <c r="F54" s="76">
-        <v>0.5</v>
-      </c>
-      <c r="G54" s="76">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>19</v>
       </c>
@@ -3997,14 +3670,8 @@
       <c r="E55" s="76">
         <v>0.05</v>
       </c>
-      <c r="F55" s="76">
-        <v>0.05</v>
-      </c>
-      <c r="G55" s="76">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
         <v>36</v>
       </c>
@@ -4020,14 +3687,8 @@
       <c r="E56" s="78">
         <v>1E-3</v>
       </c>
-      <c r="F56" s="78">
-        <v>1E-3</v>
-      </c>
-      <c r="G56" s="78">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="16" t="s">
         <v>379</v>
       </c>
@@ -4043,14 +3704,8 @@
       <c r="E57" s="76">
         <v>0</v>
       </c>
-      <c r="F57" s="76">
-        <v>0</v>
-      </c>
-      <c r="G57" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
         <v>37</v>
       </c>
@@ -4066,14 +3721,8 @@
       <c r="E58" s="76">
         <v>1E-4</v>
       </c>
-      <c r="F58" s="76">
-        <v>1E-4</v>
-      </c>
-      <c r="G58" s="76">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
         <v>38</v>
       </c>
@@ -4089,14 +3738,8 @@
       <c r="E59" s="76">
         <v>1E-4</v>
       </c>
-      <c r="F59" s="76">
-        <v>1E-4</v>
-      </c>
-      <c r="G59" s="76">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="18" t="s">
         <v>39</v>
       </c>
@@ -4112,14 +3755,8 @@
       <c r="E60" s="76">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="F60" s="76">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="G60" s="76">
-        <v>6.9999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="18" t="s">
         <v>40</v>
       </c>
@@ -4135,14 +3772,8 @@
       <c r="E61" s="76">
         <v>1.22E-4</v>
       </c>
-      <c r="F61" s="76">
-        <v>1.22E-4</v>
-      </c>
-      <c r="G61" s="76">
-        <v>1.22E-4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="18" t="s">
         <v>206</v>
       </c>
@@ -4158,14 +3789,8 @@
       <c r="E62" s="76">
         <v>1</v>
       </c>
-      <c r="F62" s="76">
-        <v>1</v>
-      </c>
-      <c r="G62" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="18" t="s">
         <v>41</v>
       </c>
@@ -4181,14 +3806,8 @@
       <c r="E63" s="76">
         <v>0.95</v>
       </c>
-      <c r="F63" s="76">
-        <v>0.95</v>
-      </c>
-      <c r="G63" s="76">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="18" t="s">
         <v>407</v>
       </c>
@@ -4204,14 +3823,8 @@
       <c r="E64" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F64" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G64" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="18" t="s">
         <v>90</v>
       </c>
@@ -4227,14 +3840,8 @@
       <c r="E65" s="76">
         <v>5</v>
       </c>
-      <c r="F65" s="76">
-        <v>5</v>
-      </c>
-      <c r="G65" s="76">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="18" t="s">
         <v>409</v>
       </c>
@@ -4250,14 +3857,8 @@
       <c r="E66" s="76" t="s">
         <v>88</v>
       </c>
-      <c r="F66" s="76" t="s">
-        <v>88</v>
-      </c>
-      <c r="G66" s="76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="18" t="s">
         <v>42</v>
       </c>
@@ -4273,14 +3874,8 @@
       <c r="E67" s="76">
         <v>50</v>
       </c>
-      <c r="F67" s="76">
-        <v>50</v>
-      </c>
-      <c r="G67" s="76">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="18" t="s">
         <v>207</v>
       </c>
@@ -4296,14 +3891,8 @@
       <c r="E68" s="77">
         <v>1453890.8941884842</v>
       </c>
-      <c r="F68" s="77">
-        <v>1453890.8941884842</v>
-      </c>
-      <c r="G68" s="77">
-        <v>1453890.8941884842</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="18" t="s">
         <v>43</v>
       </c>
@@ -4319,14 +3908,8 @@
       <c r="E69" s="77">
         <v>1.3888888888888888E-5</v>
       </c>
-      <c r="F69" s="77">
-        <v>1.3888888888888888E-5</v>
-      </c>
-      <c r="G69" s="77">
-        <v>1.3888888888888888E-5</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="18" t="s">
         <v>44</v>
       </c>
@@ -4342,14 +3925,8 @@
       <c r="E70" s="77">
         <v>6.5011574074074071E-4</v>
       </c>
-      <c r="F70" s="77">
-        <v>6.5011574074074071E-4</v>
-      </c>
-      <c r="G70" s="77">
-        <v>6.5011574074074071E-4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="18" t="s">
         <v>45</v>
       </c>
@@ -4365,14 +3942,8 @@
       <c r="E71" s="76">
         <v>4.7400000000000003E-3</v>
       </c>
-      <c r="F71" s="76">
-        <v>4.7400000000000003E-3</v>
-      </c>
-      <c r="G71" s="76">
-        <v>4.7400000000000003E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="18" t="s">
         <v>46</v>
       </c>
@@ -4388,14 +3959,8 @@
       <c r="E72" s="77">
         <v>282528</v>
       </c>
-      <c r="F72" s="77">
-        <v>282528</v>
-      </c>
-      <c r="G72" s="77">
-        <v>282528</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="18" t="s">
         <v>47</v>
       </c>
@@ -4411,14 +3976,8 @@
       <c r="E73" s="76">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F73" s="76">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="G73" s="76">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="18" t="s">
         <v>48</v>
       </c>
@@ -4434,14 +3993,8 @@
       <c r="E74" s="81">
         <v>0.16</v>
       </c>
-      <c r="F74" s="81">
-        <v>0.16</v>
-      </c>
-      <c r="G74" s="81">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="18" t="s">
         <v>49</v>
       </c>
@@ -4457,14 +4010,8 @@
       <c r="E75" s="76">
         <v>0</v>
       </c>
-      <c r="F75" s="76">
-        <v>0</v>
-      </c>
-      <c r="G75" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="34" t="s">
         <v>50</v>
       </c>
@@ -4480,14 +4027,8 @@
       <c r="E76" s="77">
         <v>745476480000</v>
       </c>
-      <c r="F76" s="77">
-        <v>745476480000</v>
-      </c>
-      <c r="G76" s="77">
-        <v>745476480000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="34" t="s">
         <v>204</v>
       </c>
@@ -4503,14 +4044,8 @@
       <c r="E77" s="76">
         <v>100</v>
       </c>
-      <c r="F77" s="76">
-        <v>100</v>
-      </c>
-      <c r="G77" s="76">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="34" t="s">
         <v>415</v>
       </c>
@@ -4526,14 +4061,8 @@
       <c r="E78" s="76" t="s">
         <v>87</v>
       </c>
-      <c r="F78" s="76" t="s">
-        <v>87</v>
-      </c>
-      <c r="G78" s="76" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="34" t="s">
         <v>400</v>
       </c>
@@ -4549,14 +4078,8 @@
       <c r="E79" s="76">
         <v>21600</v>
       </c>
-      <c r="F79" s="76">
-        <v>21600</v>
-      </c>
-      <c r="G79" s="76">
-        <v>21600</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="34" t="s">
         <v>411</v>
       </c>
@@ -4572,14 +4095,8 @@
       <c r="E80" s="76">
         <v>0.5</v>
       </c>
-      <c r="F80" s="76">
-        <v>0.5</v>
-      </c>
-      <c r="G80" s="76">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="34" t="s">
         <v>401</v>
       </c>
@@ -4595,14 +4112,8 @@
       <c r="E81" s="76">
         <v>60479.999999999993</v>
       </c>
-      <c r="F81" s="76">
-        <v>60479.999999999993</v>
-      </c>
-      <c r="G81" s="76">
-        <v>60479.999999999993</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="34" t="s">
         <v>412</v>
       </c>
@@ -4618,14 +4129,8 @@
       <c r="E82" s="76">
         <v>0.85</v>
       </c>
-      <c r="F82" s="76">
-        <v>0.85</v>
-      </c>
-      <c r="G82" s="76">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="34" t="s">
         <v>402</v>
       </c>
@@ -4641,14 +4146,8 @@
       <c r="E83" s="76">
         <v>518400</v>
       </c>
-      <c r="F83" s="76">
-        <v>518400</v>
-      </c>
-      <c r="G83" s="76">
-        <v>518400</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="34" t="s">
         <v>413</v>
       </c>
@@ -4664,14 +4163,8 @@
       <c r="E84" s="76">
         <v>5184000</v>
       </c>
-      <c r="F84" s="76">
-        <v>5184000</v>
-      </c>
-      <c r="G84" s="76">
-        <v>5184000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="18" t="s">
         <v>51</v>
       </c>
@@ -4687,14 +4180,8 @@
       <c r="E85" s="78">
         <v>50000</v>
       </c>
-      <c r="F85" s="78">
-        <v>50000</v>
-      </c>
-      <c r="G85" s="78">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="18" t="s">
         <v>52</v>
       </c>
@@ -4710,14 +4197,8 @@
       <c r="E86" s="76">
         <v>140000</v>
       </c>
-      <c r="F86" s="76">
-        <v>140000</v>
-      </c>
-      <c r="G86" s="76">
-        <v>140000</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="18" t="s">
         <v>53</v>
       </c>
@@ -4733,14 +4214,8 @@
       <c r="E87" s="77">
         <v>3.6636136999999999E-2</v>
       </c>
-      <c r="F87" s="77">
-        <v>3.6636136999999999E-2</v>
-      </c>
-      <c r="G87" s="77">
-        <v>3.6636136999999999E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="18" t="s">
         <v>54</v>
       </c>
@@ -4756,14 +4231,8 @@
       <c r="E88" s="76">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="F88" s="76">
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="G88" s="76">
-        <v>4.4999999999999997E-3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="18" t="s">
         <v>55</v>
       </c>
@@ -4779,14 +4248,8 @@
       <c r="E89" s="76">
         <v>0.05</v>
       </c>
-      <c r="F89" s="76">
-        <v>0.05</v>
-      </c>
-      <c r="G89" s="76">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="18" t="s">
         <v>496</v>
       </c>
@@ -4802,14 +4265,8 @@
       <c r="E90" s="76">
         <v>0</v>
       </c>
-      <c r="F90" s="76">
-        <v>0</v>
-      </c>
-      <c r="G90" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="20" t="s">
         <v>213</v>
       </c>
@@ -4825,14 +4282,8 @@
       <c r="E91" s="76">
         <v>6.0000000000000002E-6</v>
       </c>
-      <c r="F91" s="76">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="G91" s="76">
-        <v>6.0000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="20" t="s">
         <v>214</v>
       </c>
@@ -4848,14 +4299,8 @@
       <c r="E92" s="76">
         <v>1E-3</v>
       </c>
-      <c r="F92" s="76">
-        <v>1E-3</v>
-      </c>
-      <c r="G92" s="76">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="20" t="s">
         <v>215</v>
       </c>
@@ -4871,14 +4316,8 @@
       <c r="E93" s="76">
         <v>374999999.99999994</v>
       </c>
-      <c r="F93" s="76">
-        <v>374999999.99999994</v>
-      </c>
-      <c r="G93" s="76">
-        <v>374999999.99999994</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="20" t="s">
         <v>216</v>
       </c>
@@ -4894,14 +4333,8 @@
       <c r="E94" s="77">
         <v>3.7037037037037038E-3</v>
       </c>
-      <c r="F94" s="77">
-        <v>3.7037037037037038E-3</v>
-      </c>
-      <c r="G94" s="77">
-        <v>3.7037037037037038E-3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="20" t="s">
         <v>217</v>
       </c>
@@ -4917,14 +4350,8 @@
       <c r="E95" s="76">
         <v>165600</v>
       </c>
-      <c r="F95" s="76">
-        <v>165600</v>
-      </c>
-      <c r="G95" s="76">
-        <v>165600</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="14" t="s">
         <v>60</v>
       </c>
@@ -4940,14 +4367,8 @@
       <c r="E96" s="76">
         <v>20</v>
       </c>
-      <c r="F96" s="76">
-        <v>20</v>
-      </c>
-      <c r="G96" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="14" t="s">
         <v>208</v>
       </c>
@@ -4963,14 +4384,8 @@
       <c r="E97" s="76">
         <v>1</v>
       </c>
-      <c r="F97" s="76">
-        <v>1</v>
-      </c>
-      <c r="G97" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="14" t="s">
         <v>59</v>
       </c>
@@ -4986,14 +4401,8 @@
       <c r="E98" s="76">
         <v>21</v>
       </c>
-      <c r="F98" s="76">
-        <v>21</v>
-      </c>
-      <c r="G98" s="76">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="24" t="s">
         <v>65</v>
       </c>
@@ -5009,14 +4418,8 @@
       <c r="E99" s="76">
         <v>0.64</v>
       </c>
-      <c r="F99" s="76">
-        <v>0.64</v>
-      </c>
-      <c r="G99" s="76">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="24" t="s">
         <v>366</v>
       </c>
@@ -5032,14 +4435,8 @@
       <c r="E100" s="76">
         <v>8</v>
       </c>
-      <c r="F100" s="76">
-        <v>8</v>
-      </c>
-      <c r="G100" s="76">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="24" t="s">
         <v>367</v>
       </c>
@@ -5055,14 +4452,8 @@
       <c r="E101" s="76">
         <v>10</v>
       </c>
-      <c r="F101" s="76">
-        <v>10</v>
-      </c>
-      <c r="G101" s="76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="24" t="s">
         <v>368</v>
       </c>
@@ -5078,14 +4469,8 @@
       <c r="E102" s="76">
         <v>8</v>
       </c>
-      <c r="F102" s="76">
-        <v>8</v>
-      </c>
-      <c r="G102" s="76">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="24" t="s">
         <v>383</v>
       </c>
@@ -5101,14 +4486,8 @@
       <c r="E103" s="76">
         <v>1</v>
       </c>
-      <c r="F103" s="76">
-        <v>1</v>
-      </c>
-      <c r="G103" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="24" t="s">
         <v>385</v>
       </c>
@@ -5124,14 +4503,8 @@
       <c r="E104" s="76">
         <v>0.5</v>
       </c>
-      <c r="F104" s="76">
-        <v>0.5</v>
-      </c>
-      <c r="G104" s="76">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="24" t="s">
         <v>387</v>
       </c>
@@ -5147,14 +4520,8 @@
       <c r="E105" s="76">
         <v>0</v>
       </c>
-      <c r="F105" s="76">
-        <v>0</v>
-      </c>
-      <c r="G105" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="24" t="s">
         <v>389</v>
       </c>
@@ -5170,14 +4537,8 @@
       <c r="E106" s="82">
         <v>1589759.9999999998</v>
       </c>
-      <c r="F106" s="82">
-        <v>1589759.9999999998</v>
-      </c>
-      <c r="G106" s="82">
-        <v>1589759.9999999998</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="24" t="s">
         <v>391</v>
       </c>
@@ -5193,14 +4554,8 @@
       <c r="E107" s="82">
         <v>455327.99999999994</v>
       </c>
-      <c r="F107" s="82">
-        <v>455327.99999999994</v>
-      </c>
-      <c r="G107" s="82">
-        <v>455327.99999999994</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="24" t="s">
         <v>393</v>
       </c>
@@ -5216,14 +4571,8 @@
       <c r="E108" s="82">
         <v>664416</v>
       </c>
-      <c r="F108" s="82">
-        <v>664416</v>
-      </c>
-      <c r="G108" s="82">
-        <v>664416</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="24" t="s">
         <v>422</v>
       </c>
@@ -5239,14 +4588,8 @@
       <c r="E109" s="82">
         <v>100</v>
       </c>
-      <c r="F109" s="82">
-        <v>100</v>
-      </c>
-      <c r="G109" s="82">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="24" t="s">
         <v>424</v>
       </c>
@@ -5262,14 +4605,8 @@
       <c r="E110" s="82">
         <v>280800</v>
       </c>
-      <c r="F110" s="82">
-        <v>280800</v>
-      </c>
-      <c r="G110" s="82">
-        <v>280800</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="24" t="s">
         <v>426</v>
       </c>
@@ -5285,14 +4622,8 @@
       <c r="E111" s="83">
         <v>1.2847222222222224E-5</v>
       </c>
-      <c r="F111" s="83">
-        <v>1.2847222222222224E-5</v>
-      </c>
-      <c r="G111" s="83">
-        <v>1.2847222222222224E-5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="24" t="s">
         <v>428</v>
       </c>
@@ -5308,14 +4639,8 @@
       <c r="E112" s="82">
         <v>90</v>
       </c>
-      <c r="F112" s="82">
-        <v>90</v>
-      </c>
-      <c r="G112" s="82">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="24" t="s">
         <v>430</v>
       </c>
@@ -5331,14 +4656,8 @@
       <c r="E113" s="82">
         <v>459648</v>
       </c>
-      <c r="F113" s="82">
-        <v>459648</v>
-      </c>
-      <c r="G113" s="82">
-        <v>459648</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="24" t="s">
         <v>432</v>
       </c>
@@ -5354,14 +4673,8 @@
       <c r="E114" s="83">
         <v>1.2847222222222224E-5</v>
       </c>
-      <c r="F114" s="83">
-        <v>1.2847222222222224E-5</v>
-      </c>
-      <c r="G114" s="83">
-        <v>1.2847222222222224E-5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="24" t="s">
         <v>395</v>
       </c>
@@ -5377,14 +4690,8 @@
       <c r="E115" s="82">
         <v>21600</v>
       </c>
-      <c r="F115" s="82">
-        <v>21600</v>
-      </c>
-      <c r="G115" s="82">
-        <v>21600</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
         <v>397</v>
       </c>
@@ -5400,14 +4707,8 @@
       <c r="E116" s="82">
         <v>43200</v>
       </c>
-      <c r="F116" s="82">
-        <v>43200</v>
-      </c>
-      <c r="G116" s="82">
-        <v>43200</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="14" t="s">
         <v>61</v>
       </c>
@@ -5423,14 +4724,8 @@
       <c r="E117" s="76">
         <v>0.8</v>
       </c>
-      <c r="F117" s="76">
-        <v>0.8</v>
-      </c>
-      <c r="G117" s="76">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="14" t="s">
         <v>62</v>
       </c>
@@ -5446,14 +4741,8 @@
       <c r="E118" s="77">
         <v>2.0833333333333335E-4</v>
       </c>
-      <c r="F118" s="77">
-        <v>2.0833333333333335E-4</v>
-      </c>
-      <c r="G118" s="77">
-        <v>2.0833333333333335E-4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="14" t="s">
         <v>63</v>
       </c>
@@ -5469,14 +4758,8 @@
       <c r="E119" s="83">
         <v>5.7899999999999998E-7</v>
       </c>
-      <c r="F119" s="83">
-        <v>5.7899999999999998E-7</v>
-      </c>
-      <c r="G119" s="83">
-        <v>5.7899999999999998E-7</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="14" t="s">
         <v>64</v>
       </c>
@@ -5492,14 +4775,8 @@
       <c r="E120" s="77">
         <v>2.0833333333333335E-4</v>
       </c>
-      <c r="F120" s="77">
-        <v>2.0833333333333335E-4</v>
-      </c>
-      <c r="G120" s="77">
-        <v>2.0833333333333335E-4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="14" t="s">
         <v>463</v>
       </c>
@@ -5515,14 +4792,8 @@
       <c r="E121" s="77">
         <v>0</v>
       </c>
-      <c r="F121" s="77">
-        <v>0</v>
-      </c>
-      <c r="G121" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="14" t="s">
         <v>464</v>
       </c>
@@ -5538,14 +4809,8 @@
       <c r="E122" s="77">
         <v>0</v>
       </c>
-      <c r="F122" s="77">
-        <v>0</v>
-      </c>
-      <c r="G122" s="77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="22" t="s">
         <v>445</v>
       </c>
@@ -5561,14 +4826,8 @@
       <c r="E123" s="84" t="s">
         <v>406</v>
       </c>
-      <c r="F123" s="84" t="s">
-        <v>406</v>
-      </c>
-      <c r="G123" s="84" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="22" t="s">
         <v>67</v>
       </c>
@@ -5584,14 +4843,8 @@
       <c r="E124" s="84" t="s">
         <v>406</v>
       </c>
-      <c r="F124" s="84" t="s">
-        <v>406</v>
-      </c>
-      <c r="G124" s="84" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="22" t="s">
         <v>459</v>
       </c>
@@ -5607,14 +4860,8 @@
       <c r="E125" s="84" t="s">
         <v>87</v>
       </c>
-      <c r="F125" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="G125" s="84" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="22" t="s">
         <v>66</v>
       </c>
@@ -5630,14 +4877,8 @@
       <c r="E126" s="78">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F126" s="78">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="G126" s="78">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="22" t="s">
         <v>441</v>
       </c>
@@ -5653,14 +4894,8 @@
       <c r="E127" s="78">
         <v>4.9999999999999999E-13</v>
       </c>
-      <c r="F127" s="78">
-        <v>4.9999999999999999E-13</v>
-      </c>
-      <c r="G127" s="78">
-        <v>4.9999999999999999E-13</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="22" t="s">
         <v>450</v>
       </c>
@@ -5676,14 +4911,8 @@
       <c r="E128" s="76">
         <v>10</v>
       </c>
-      <c r="F128" s="76">
-        <v>10</v>
-      </c>
-      <c r="G128" s="76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="22" t="s">
         <v>451</v>
       </c>
@@ -5699,14 +4928,8 @@
       <c r="E129" s="76">
         <v>-0.04</v>
       </c>
-      <c r="F129" s="76">
-        <v>-0.04</v>
-      </c>
-      <c r="G129" s="76">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="22" t="s">
         <v>452</v>
       </c>
@@ -5722,14 +4945,8 @@
       <c r="E130" s="76">
         <v>2.9</v>
       </c>
-      <c r="F130" s="76">
-        <v>2.9</v>
-      </c>
-      <c r="G130" s="76">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="22" t="s">
         <v>453</v>
       </c>
@@ -5745,14 +4962,8 @@
       <c r="E131" s="76">
         <v>1</v>
       </c>
-      <c r="F131" s="76">
-        <v>1</v>
-      </c>
-      <c r="G131" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="22" t="s">
         <v>444</v>
       </c>
@@ -5768,14 +4979,8 @@
       <c r="E132" s="78">
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="F132" s="78">
-        <v>1.9999999999999999E-7</v>
-      </c>
-      <c r="G132" s="78">
-        <v>1.9999999999999999E-7</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="22" t="s">
         <v>232</v>
       </c>
@@ -5791,14 +4996,8 @@
       <c r="E133" s="76">
         <v>10</v>
       </c>
-      <c r="F133" s="76">
-        <v>10</v>
-      </c>
-      <c r="G133" s="76">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="22" t="s">
         <v>233</v>
       </c>
@@ -5814,14 +5013,8 @@
       <c r="E134" s="76">
         <v>-0.04</v>
       </c>
-      <c r="F134" s="76">
-        <v>-0.04</v>
-      </c>
-      <c r="G134" s="76">
-        <v>-0.04</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="22" t="s">
         <v>234</v>
       </c>
@@ -5837,14 +5030,8 @@
       <c r="E135" s="76">
         <v>2.9</v>
       </c>
-      <c r="F135" s="76">
-        <v>2.9</v>
-      </c>
-      <c r="G135" s="76">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="22" t="s">
         <v>235</v>
       </c>
@@ -5860,14 +5047,8 @@
       <c r="E136" s="76">
         <v>1</v>
       </c>
-      <c r="F136" s="76">
-        <v>1</v>
-      </c>
-      <c r="G136" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="22" t="s">
         <v>69</v>
       </c>
@@ -5883,14 +5064,8 @@
       <c r="E137" s="76">
         <v>0</v>
       </c>
-      <c r="F137" s="76">
-        <v>0</v>
-      </c>
-      <c r="G137" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="22" t="s">
         <v>70</v>
       </c>
@@ -5906,14 +5081,8 @@
       <c r="E138" s="78">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="F138" s="78">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="G138" s="78">
-        <v>5.0000000000000004E-6</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="24" t="s">
         <v>56</v>
       </c>
@@ -5929,14 +5098,8 @@
       <c r="E139" s="76">
         <v>0</v>
       </c>
-      <c r="F139" s="76">
-        <v>0</v>
-      </c>
-      <c r="G139" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="24" t="s">
         <v>57</v>
       </c>
@@ -5952,14 +5115,8 @@
       <c r="E140" s="76">
         <v>2E-3</v>
       </c>
-      <c r="F140" s="76">
-        <v>2E-3</v>
-      </c>
-      <c r="G140" s="76">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="24" t="s">
         <v>58</v>
       </c>
@@ -5975,14 +5132,8 @@
       <c r="E141" s="78">
         <v>3.9999999999999998E-6</v>
       </c>
-      <c r="F141" s="78">
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="G141" s="78">
-        <v>3.9999999999999998E-6</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="24" t="s">
         <v>71</v>
       </c>
@@ -5998,14 +5149,8 @@
       <c r="E142" s="78">
         <v>3.7699999999999999E-10</v>
       </c>
-      <c r="F142" s="78">
-        <v>3.7699999999999999E-10</v>
-      </c>
-      <c r="G142" s="78">
-        <v>3.7699999999999999E-10</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="24" t="s">
         <v>236</v>
       </c>
@@ -6021,14 +5166,8 @@
       <c r="E143" s="76">
         <v>20</v>
       </c>
-      <c r="F143" s="76">
-        <v>20</v>
-      </c>
-      <c r="G143" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="24" t="s">
         <v>237</v>
       </c>
@@ -6044,14 +5183,8 @@
       <c r="E144" s="76">
         <v>-0.06</v>
       </c>
-      <c r="F144" s="76">
-        <v>-0.06</v>
-      </c>
-      <c r="G144" s="76">
-        <v>-0.06</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
         <v>238</v>
       </c>
@@ -6067,14 +5200,8 @@
       <c r="E145" s="76">
         <v>0.89100000000000001</v>
       </c>
-      <c r="F145" s="76">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="G145" s="76">
-        <v>0.89100000000000001</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
         <v>239</v>
       </c>
@@ -6090,14 +5217,8 @@
       <c r="E146" s="76">
         <v>1</v>
       </c>
-      <c r="F146" s="76">
-        <v>1</v>
-      </c>
-      <c r="G146" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="24" t="s">
         <v>72</v>
       </c>
@@ -6113,14 +5234,8 @@
       <c r="E147" s="78">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="F147" s="78">
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="G147" s="78">
-        <v>4.0000000000000003E-5</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="14" t="s">
         <v>73</v>
       </c>
@@ -6136,14 +5251,8 @@
       <c r="E148" s="78">
         <v>5.8333333333333335E-9</v>
       </c>
-      <c r="F148" s="78">
-        <v>5.8333333333333335E-9</v>
-      </c>
-      <c r="G148" s="78">
-        <v>5.8333333333333335E-9</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="14" t="s">
         <v>240</v>
       </c>
@@ -6159,14 +5268,8 @@
       <c r="E149" s="76">
         <v>20</v>
       </c>
-      <c r="F149" s="76">
-        <v>20</v>
-      </c>
-      <c r="G149" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="14" t="s">
         <v>241</v>
       </c>
@@ -6182,14 +5285,8 @@
       <c r="E150" s="76">
         <v>-0.06</v>
       </c>
-      <c r="F150" s="76">
-        <v>-0.06</v>
-      </c>
-      <c r="G150" s="76">
-        <v>-0.06</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="14" t="s">
         <v>242</v>
       </c>
@@ -6205,14 +5302,8 @@
       <c r="E151" s="76">
         <v>0.89100000000000001</v>
       </c>
-      <c r="F151" s="76">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="G151" s="76">
-        <v>0.89100000000000001</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="14" t="s">
         <v>243</v>
       </c>
@@ -6228,14 +5319,8 @@
       <c r="E152" s="76">
         <v>1</v>
       </c>
-      <c r="F152" s="76">
-        <v>1</v>
-      </c>
-      <c r="G152" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="14" t="s">
         <v>74</v>
       </c>
@@ -6251,14 +5336,8 @@
       <c r="E153" s="78">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="F153" s="78">
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="G153" s="78">
-        <v>4.0000000000000003E-5</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="10" t="s">
         <v>75</v>
       </c>
@@ -6274,14 +5353,8 @@
       <c r="E154" s="78">
         <v>4.0000000000000001E-8</v>
       </c>
-      <c r="F154" s="78">
-        <v>4.0000000000000001E-8</v>
-      </c>
-      <c r="G154" s="78">
-        <v>4.0000000000000001E-8</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="10" t="s">
         <v>218</v>
       </c>
@@ -6297,14 +5370,8 @@
       <c r="E155" s="76">
         <v>20</v>
       </c>
-      <c r="F155" s="76">
-        <v>20</v>
-      </c>
-      <c r="G155" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="10" t="s">
         <v>219</v>
       </c>
@@ -6320,14 +5387,8 @@
       <c r="E156" s="76">
         <v>-4.4200000000000003E-2</v>
       </c>
-      <c r="F156" s="76">
-        <v>-4.4200000000000003E-2</v>
-      </c>
-      <c r="G156" s="76">
-        <v>-4.4200000000000003E-2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="10" t="s">
         <v>220</v>
       </c>
@@ -6343,14 +5404,8 @@
       <c r="E157" s="76">
         <v>1.55</v>
       </c>
-      <c r="F157" s="76">
-        <v>1.55</v>
-      </c>
-      <c r="G157" s="76">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="10" t="s">
         <v>221</v>
       </c>
@@ -6366,14 +5421,8 @@
       <c r="E158" s="76">
         <v>1</v>
       </c>
-      <c r="F158" s="76">
-        <v>1</v>
-      </c>
-      <c r="G158" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="10" t="s">
         <v>76</v>
       </c>
@@ -6389,14 +5438,8 @@
       <c r="E159" s="76">
         <v>2.7799999999999998E-4</v>
       </c>
-      <c r="F159" s="76">
-        <v>2.7799999999999998E-4</v>
-      </c>
-      <c r="G159" s="76">
-        <v>2.7799999999999998E-4</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="26" t="s">
         <v>78</v>
       </c>
@@ -6412,14 +5455,8 @@
       <c r="E160" s="78">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="F160" s="78">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="G160" s="78">
-        <v>2.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="26" t="s">
         <v>245</v>
       </c>
@@ -6435,14 +5472,8 @@
       <c r="E161" s="76">
         <v>20</v>
       </c>
-      <c r="F161" s="76">
-        <v>20</v>
-      </c>
-      <c r="G161" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="26" t="s">
         <v>246</v>
       </c>
@@ -6458,14 +5489,8 @@
       <c r="E162" s="76">
         <v>0</v>
       </c>
-      <c r="F162" s="76">
-        <v>0</v>
-      </c>
-      <c r="G162" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="26" t="s">
         <v>247</v>
       </c>
@@ -6481,14 +5506,8 @@
       <c r="E163" s="76">
         <v>1</v>
       </c>
-      <c r="F163" s="76">
-        <v>1</v>
-      </c>
-      <c r="G163" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" s="26" t="s">
         <v>248</v>
       </c>
@@ -6504,14 +5523,8 @@
       <c r="E164" s="76">
         <v>0</v>
       </c>
-      <c r="F164" s="76">
-        <v>0</v>
-      </c>
-      <c r="G164" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="26" t="s">
         <v>79</v>
       </c>
@@ -6527,14 +5540,8 @@
       <c r="E165" s="76">
         <v>0.4</v>
       </c>
-      <c r="F165" s="76">
-        <v>0.4</v>
-      </c>
-      <c r="G165" s="76">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="32" t="s">
         <v>80</v>
       </c>
@@ -6550,14 +5557,8 @@
       <c r="E166" s="78">
         <v>2.0000000000000001E-9</v>
       </c>
-      <c r="F166" s="78">
-        <v>2.0000000000000001E-9</v>
-      </c>
-      <c r="G166" s="78">
-        <v>2.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="32" t="s">
         <v>249</v>
       </c>
@@ -6573,14 +5574,8 @@
       <c r="E167" s="76">
         <v>25</v>
       </c>
-      <c r="F167" s="76">
-        <v>25</v>
-      </c>
-      <c r="G167" s="76">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="32" t="s">
         <v>250</v>
       </c>
@@ -6596,14 +5591,8 @@
       <c r="E168" s="76">
         <v>0</v>
       </c>
-      <c r="F168" s="76">
-        <v>0</v>
-      </c>
-      <c r="G168" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="32" t="s">
         <v>251</v>
       </c>
@@ -6619,14 +5608,8 @@
       <c r="E169" s="76">
         <v>3.98</v>
       </c>
-      <c r="F169" s="76">
-        <v>3.98</v>
-      </c>
-      <c r="G169" s="76">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="32" t="s">
         <v>252</v>
       </c>
@@ -6642,14 +5625,8 @@
       <c r="E170" s="76">
         <v>1</v>
       </c>
-      <c r="F170" s="76">
-        <v>1</v>
-      </c>
-      <c r="G170" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="32" t="s">
         <v>81</v>
       </c>
@@ -6665,14 +5642,8 @@
       <c r="E171" s="77">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="F171" s="77">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="G171" s="77">
-        <v>5.0000000000000004E-6</v>
-      </c>
-    </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
         <v>253</v>
       </c>
@@ -6688,14 +5659,8 @@
       <c r="E172" s="78">
         <v>1E-8</v>
       </c>
-      <c r="F172" s="78">
-        <v>1E-8</v>
-      </c>
-      <c r="G172" s="78">
-        <v>1E-8</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" s="12" t="s">
         <v>254</v>
       </c>
@@ -6711,14 +5676,8 @@
       <c r="E173" s="76">
         <v>20</v>
       </c>
-      <c r="F173" s="76">
-        <v>20</v>
-      </c>
-      <c r="G173" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="12" t="s">
         <v>255</v>
       </c>
@@ -6734,14 +5693,8 @@
       <c r="E174" s="76">
         <v>0</v>
       </c>
-      <c r="F174" s="76">
-        <v>0</v>
-      </c>
-      <c r="G174" s="76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="12" t="s">
         <v>256</v>
       </c>
@@ -6757,14 +5710,8 @@
       <c r="E175" s="76">
         <v>2</v>
       </c>
-      <c r="F175" s="76">
-        <v>2</v>
-      </c>
-      <c r="G175" s="76">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
         <v>257</v>
       </c>
@@ -6780,14 +5727,8 @@
       <c r="E176" s="76">
         <v>1</v>
       </c>
-      <c r="F176" s="76">
-        <v>1</v>
-      </c>
-      <c r="G176" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" s="12" t="s">
         <v>258</v>
       </c>
@@ -6803,14 +5744,8 @@
       <c r="E177" s="77">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="F177" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-      <c r="G177" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="12" t="s">
         <v>259</v>
       </c>
@@ -6826,14 +5761,8 @@
       <c r="E178" s="76">
         <v>1</v>
       </c>
-      <c r="F178" s="76">
-        <v>1</v>
-      </c>
-      <c r="G178" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="28" t="s">
         <v>260</v>
       </c>
@@ -6849,14 +5778,8 @@
       <c r="E179" s="76">
         <v>2.3533050791148899E-8</v>
       </c>
-      <c r="F179" s="76">
-        <v>2.3533050791148899E-8</v>
-      </c>
-      <c r="G179" s="76">
-        <v>2.3533050791148899E-8</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="28" t="s">
         <v>261</v>
       </c>
@@ -6872,14 +5795,8 @@
       <c r="E180" s="76">
         <v>20</v>
       </c>
-      <c r="F180" s="76">
-        <v>20</v>
-      </c>
-      <c r="G180" s="76">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="28" t="s">
         <v>262</v>
       </c>
@@ -6895,14 +5812,8 @@
       <c r="E181" s="76">
         <v>-0.187</v>
       </c>
-      <c r="F181" s="76">
-        <v>-0.187</v>
-      </c>
-      <c r="G181" s="76">
-        <v>-0.187</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="28" t="s">
         <v>263</v>
       </c>
@@ -6918,14 +5829,8 @@
       <c r="E182" s="76">
         <v>2.48</v>
       </c>
-      <c r="F182" s="76">
-        <v>2.48</v>
-      </c>
-      <c r="G182" s="76">
-        <v>2.48</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="28" t="s">
         <v>264</v>
       </c>
@@ -6941,14 +5846,8 @@
       <c r="E183" s="76">
         <v>1</v>
       </c>
-      <c r="F183" s="76">
-        <v>1</v>
-      </c>
-      <c r="G183" s="76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="28" t="s">
         <v>265</v>
       </c>
@@ -6964,14 +5863,8 @@
       <c r="E184" s="76">
         <v>6.1060227588121015E-4</v>
       </c>
-      <c r="F184" s="76">
-        <v>6.1060227588121015E-4</v>
-      </c>
-      <c r="G184" s="76">
-        <v>6.1060227588121015E-4</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="24" t="s">
         <v>266</v>
       </c>
@@ -6987,14 +5880,8 @@
       <c r="E185" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-      <c r="F185" s="85">
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="G185" s="85">
-        <v>3.9999999999999998E-7</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="24" t="s">
         <v>267</v>
       </c>
@@ -7010,14 +5897,8 @@
       <c r="E186" s="85">
         <v>25</v>
       </c>
-      <c r="F186" s="85">
-        <v>25</v>
-      </c>
-      <c r="G186" s="85">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="24" t="s">
         <v>268</v>
       </c>
@@ -7033,14 +5914,8 @@
       <c r="E187" s="85">
         <v>0</v>
       </c>
-      <c r="F187" s="85">
-        <v>0</v>
-      </c>
-      <c r="G187" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="24" t="s">
         <v>269</v>
       </c>
@@ -7056,14 +5931,8 @@
       <c r="E188" s="85">
         <v>3.98</v>
       </c>
-      <c r="F188" s="85">
-        <v>3.98</v>
-      </c>
-      <c r="G188" s="85">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="24" t="s">
         <v>270</v>
       </c>
@@ -7079,14 +5948,8 @@
       <c r="E189" s="85">
         <v>1</v>
       </c>
-      <c r="F189" s="85">
-        <v>1</v>
-      </c>
-      <c r="G189" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="24" t="s">
         <v>271</v>
       </c>
@@ -7102,14 +5965,8 @@
       <c r="E190" s="77">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="F190" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-      <c r="G190" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="8" t="s">
         <v>272</v>
       </c>
@@ -7125,14 +5982,8 @@
       <c r="E191" s="85">
         <v>3.9999999999999998E-7</v>
       </c>
-      <c r="F191" s="85">
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="G191" s="85">
-        <v>3.9999999999999998E-7</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="8" t="s">
         <v>273</v>
       </c>
@@ -7148,14 +5999,8 @@
       <c r="E192" s="85">
         <v>25</v>
       </c>
-      <c r="F192" s="85">
-        <v>25</v>
-      </c>
-      <c r="G192" s="85">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="8" t="s">
         <v>274</v>
       </c>
@@ -7171,14 +6016,8 @@
       <c r="E193" s="85">
         <v>0</v>
       </c>
-      <c r="F193" s="85">
-        <v>0</v>
-      </c>
-      <c r="G193" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="8" t="s">
         <v>275</v>
       </c>
@@ -7194,14 +6033,8 @@
       <c r="E194" s="85">
         <v>3.98</v>
       </c>
-      <c r="F194" s="85">
-        <v>3.98</v>
-      </c>
-      <c r="G194" s="85">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="8" t="s">
         <v>276</v>
       </c>
@@ -7217,14 +6050,8 @@
       <c r="E195" s="85">
         <v>1</v>
       </c>
-      <c r="F195" s="85">
-        <v>1</v>
-      </c>
-      <c r="G195" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="8" t="s">
         <v>277</v>
       </c>
@@ -7240,14 +6067,8 @@
       <c r="E196" s="77">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="F196" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-      <c r="G196" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="30" t="s">
         <v>278</v>
       </c>
@@ -7263,14 +6084,8 @@
       <c r="E197" s="85">
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="F197" s="85">
-        <v>1.9999999999999999E-7</v>
-      </c>
-      <c r="G197" s="85">
-        <v>1.9999999999999999E-7</v>
-      </c>
-    </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="30" t="s">
         <v>279</v>
       </c>
@@ -7286,14 +6101,8 @@
       <c r="E198" s="85">
         <v>25</v>
       </c>
-      <c r="F198" s="85">
-        <v>25</v>
-      </c>
-      <c r="G198" s="85">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="30" t="s">
         <v>280</v>
       </c>
@@ -7309,14 +6118,8 @@
       <c r="E199" s="85">
         <v>0</v>
       </c>
-      <c r="F199" s="85">
-        <v>0</v>
-      </c>
-      <c r="G199" s="85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="30" t="s">
         <v>281</v>
       </c>
@@ -7332,14 +6135,8 @@
       <c r="E200" s="85">
         <v>3.98</v>
       </c>
-      <c r="F200" s="85">
-        <v>3.98</v>
-      </c>
-      <c r="G200" s="85">
-        <v>3.98</v>
-      </c>
-    </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="30" t="s">
         <v>282</v>
       </c>
@@ -7355,14 +6152,8 @@
       <c r="E201" s="85">
         <v>1</v>
       </c>
-      <c r="F201" s="85">
-        <v>1</v>
-      </c>
-      <c r="G201" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="30" t="s">
         <v>283</v>
       </c>
@@ -7378,14 +6169,8 @@
       <c r="E202" s="77">
         <v>2.5000000000000002E-6</v>
       </c>
-      <c r="F202" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-      <c r="G202" s="77">
-        <v>2.5000000000000002E-6</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="73" t="s">
         <v>361</v>
       </c>
@@ -7401,17 +6186,9 @@
       <c r="E203" s="86" t="s">
         <v>482</v>
       </c>
-      <c r="F203" s="86" t="s">
-        <v>482</v>
-      </c>
-      <c r="G203" s="86" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E204" s="38"/>
-      <c r="F204" s="38"/>
-      <c r="G204" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
After correcting an error in "Root exchange surface" in the output file
</commit_message>
<xml_diff>
--- a/tutorial/inputs/scenarios_list.xlsx
+++ b/tutorial/inputs/scenarios_list.xlsx
@@ -2721,10 +2721,10 @@
   <dimension ref="A1:E204"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B177" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2834,8 +2834,8 @@
       <c r="D6" s="55">
         <v>60</v>
       </c>
-      <c r="E6" s="76">
-        <v>180</v>
+      <c r="E6" s="88">
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>